<commit_message>
updates to santa clara and debate
</commit_message>
<xml_diff>
--- a/debate/US infection survey by PureProfile.xlsx
+++ b/debate/US infection survey by PureProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185E4DB5-024A-41E2-9D52-F465D48C76AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE2CBFD-6732-41E5-8B5E-4113DAFF1952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="1530" windowWidth="25185" windowHeight="14070" activeTab="3" xr2:uid="{FCA3AE10-4DB2-421F-A7BD-1B8FCB9CB7F6}"/>
+    <workbookView xWindow="3630" yWindow="2490" windowWidth="22860" windowHeight="14070" xr2:uid="{FCA3AE10-4DB2-421F-A7BD-1B8FCB9CB7F6}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="48" r:id="rId5"/>
+    <pivotCache cacheId="29" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2341,9 +2341,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15562,7 +15562,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6712B143-757A-428A-A6F1-6ED1D5425A49}" name="PivotTable1" cacheId="48" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6712B143-757A-428A-A6F1-6ED1D5425A49}" name="PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="24">
     <pivotField showAll="0"/>
@@ -15996,8 +15996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE675D50-5491-46E1-8469-93C2F4095663}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16046,13 +16046,13 @@
       <c r="A5" s="3">
         <v>0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="6">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>4</v>
       </c>
       <c r="F5">
@@ -16068,13 +16068,13 @@
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>41</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="6">
         <v>15</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>25</v>
       </c>
       <c r="F6">
@@ -16090,13 +16090,13 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>124</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="6">
         <v>49</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>79</v>
       </c>
       <c r="F7">
@@ -16112,13 +16112,13 @@
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>93</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="6">
         <v>42</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>72</v>
       </c>
       <c r="F8">
@@ -16134,13 +16134,13 @@
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>42</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="6">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>29</v>
       </c>
       <c r="F9">
@@ -16156,13 +16156,13 @@
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>53</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="6">
         <v>26</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>41</v>
       </c>
       <c r="F10">
@@ -16178,13 +16178,13 @@
       <c r="A11" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>362</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="6">
         <v>155</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>250</v>
       </c>
       <c r="F11">
@@ -16219,7 +16219,7 @@
     <col min="3" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="14" max="14" width="24.42578125" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="5" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16266,7 +16266,7 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>599</v>
       </c>
       <c r="P1" t="s">
@@ -16343,7 +16343,7 @@
       <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <f>IF(P2&lt;&gt;"", VLOOKUP(P2, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -16415,7 +16415,7 @@
       <c r="N3" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <f>IF(P3&lt;&gt;"", VLOOKUP(P3, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -16487,7 +16487,7 @@
       <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <f>IF(P4&lt;&gt;"", VLOOKUP(P4, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -16556,7 +16556,7 @@
       <c r="M5" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <f>IF(P5&lt;&gt;"", VLOOKUP(P5, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -16622,7 +16622,7 @@
       <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <f>IF(P6&lt;&gt;"", VLOOKUP(P6, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -16691,7 +16691,7 @@
       <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <f>IF(P7&lt;&gt;"", VLOOKUP(P7, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -16760,7 +16760,7 @@
       <c r="M8" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="5">
         <f>IF(P8&lt;&gt;"", VLOOKUP(P8, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -16826,7 +16826,7 @@
       <c r="M9" t="s">
         <v>50</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <f>IF(P9&lt;&gt;"", VLOOKUP(P9, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -16895,7 +16895,7 @@
       <c r="N10" t="s">
         <v>68</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="5">
         <f>IF(P10&lt;&gt;"", VLOOKUP(P10, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -16958,7 +16958,7 @@
       <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="5">
         <f>IF(P11&lt;&gt;"", VLOOKUP(P11, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17018,7 +17018,7 @@
       <c r="M12" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="5">
         <f>IF(P12&lt;&gt;"", VLOOKUP(P12, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17087,7 +17087,7 @@
       <c r="M13" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <f>IF(P13&lt;&gt;"", VLOOKUP(P13, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17153,7 +17153,7 @@
       <c r="M14" t="s">
         <v>50</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="5">
         <f>IF(P14&lt;&gt;"", VLOOKUP(P14, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17219,7 +17219,7 @@
       <c r="M15" t="s">
         <v>50</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="5">
         <f>IF(P15&lt;&gt;"", VLOOKUP(P15, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17285,7 +17285,7 @@
       <c r="M16" t="s">
         <v>50</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="5">
         <f>IF(P16&lt;&gt;"", VLOOKUP(P16, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17354,7 +17354,7 @@
       <c r="N17" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="5">
         <f>IF(P17&lt;&gt;"", VLOOKUP(P17, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="N18" t="s">
         <v>68</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="5">
         <f>IF(P18&lt;&gt;"", VLOOKUP(P18, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17489,7 +17489,7 @@
       <c r="M19" t="s">
         <v>25</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <f>IF(P19&lt;&gt;"", VLOOKUP(P19, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17561,7 +17561,7 @@
       <c r="N20" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="5">
         <f>IF(P20&lt;&gt;"", VLOOKUP(P20, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17624,7 +17624,7 @@
       <c r="M21" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="5">
         <f>IF(P21&lt;&gt;"", VLOOKUP(P21, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17684,7 +17684,7 @@
       <c r="M22" t="s">
         <v>50</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="5">
         <f>IF(P22&lt;&gt;"", VLOOKUP(P22, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17744,7 +17744,7 @@
       <c r="M23" t="s">
         <v>50</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="5">
         <f>IF(P23&lt;&gt;"", VLOOKUP(P23, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -17804,7 +17804,7 @@
       <c r="M24" t="s">
         <v>25</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="5">
         <f>IF(P24&lt;&gt;"", VLOOKUP(P24, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17876,7 +17876,7 @@
       <c r="N25" t="s">
         <v>28</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="5">
         <f>IF(P25&lt;&gt;"", VLOOKUP(P25, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -17939,7 +17939,7 @@
       <c r="M26" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="5">
         <f>IF(P26&lt;&gt;"", VLOOKUP(P26, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -18008,7 +18008,7 @@
       <c r="M27" t="s">
         <v>50</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="5">
         <f>IF(P27&lt;&gt;"", VLOOKUP(P27, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18074,7 +18074,7 @@
       <c r="M28" t="s">
         <v>50</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="5">
         <f>IF(P28&lt;&gt;"", VLOOKUP(P28, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18143,7 +18143,7 @@
       <c r="N29" t="s">
         <v>28</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="5">
         <f>IF(P29&lt;&gt;"", VLOOKUP(P29, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -18215,7 +18215,7 @@
       <c r="N30" t="s">
         <v>28</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="5">
         <f>IF(P30&lt;&gt;"", VLOOKUP(P30, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -18284,7 +18284,7 @@
       <c r="M31" t="s">
         <v>50</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="5">
         <f>IF(P31&lt;&gt;"", VLOOKUP(P31, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18350,7 +18350,7 @@
       <c r="M32" t="s">
         <v>50</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="5">
         <f>IF(P32&lt;&gt;"", VLOOKUP(P32, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18410,7 +18410,7 @@
       <c r="M33" t="s">
         <v>50</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="5">
         <f>IF(P33&lt;&gt;"", VLOOKUP(P33, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18470,7 +18470,7 @@
       <c r="M34" t="s">
         <v>50</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
         <f>IF(P34&lt;&gt;"", VLOOKUP(P34, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18530,7 +18530,7 @@
       <c r="M35" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="5">
         <f>IF(P35&lt;&gt;"", VLOOKUP(P35, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18596,7 +18596,7 @@
       <c r="M36" t="s">
         <v>50</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
         <f>IF(P36&lt;&gt;"", VLOOKUP(P36, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18665,7 +18665,7 @@
       <c r="N37" t="s">
         <v>28</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="5">
         <f>IF(P37&lt;&gt;"", VLOOKUP(P37, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -18734,7 +18734,7 @@
       <c r="M38" t="s">
         <v>50</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="5">
         <f>IF(P38&lt;&gt;"", VLOOKUP(P38, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18803,7 +18803,7 @@
       <c r="N39" t="s">
         <v>28</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="5">
         <f>IF(P39&lt;&gt;"", VLOOKUP(P39, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -18872,7 +18872,7 @@
       <c r="M40" t="s">
         <v>50</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="5">
         <f>IF(P40&lt;&gt;"", VLOOKUP(P40, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18938,7 +18938,7 @@
       <c r="M41" t="s">
         <v>50</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="5">
         <f>IF(P41&lt;&gt;"", VLOOKUP(P41, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -18998,7 +18998,7 @@
       <c r="M42" t="s">
         <v>50</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="5">
         <f>IF(P42&lt;&gt;"", VLOOKUP(P42, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19064,7 +19064,7 @@
       <c r="M43" t="s">
         <v>50</v>
       </c>
-      <c r="O43" s="6">
+      <c r="O43" s="5">
         <f>IF(P43&lt;&gt;"", VLOOKUP(P43, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19130,7 +19130,7 @@
       <c r="M44" t="s">
         <v>50</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="5">
         <f>IF(P44&lt;&gt;"", VLOOKUP(P44, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="M45" t="s">
         <v>50</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="5">
         <f>IF(P45&lt;&gt;"", VLOOKUP(P45, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19256,7 +19256,7 @@
       <c r="M46" t="s">
         <v>25</v>
       </c>
-      <c r="O46" s="6">
+      <c r="O46" s="5">
         <f>IF(P46&lt;&gt;"", VLOOKUP(P46, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -19325,7 +19325,7 @@
       <c r="M47" t="s">
         <v>50</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="5">
         <f>IF(P47&lt;&gt;"", VLOOKUP(P47, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19394,7 +19394,7 @@
       <c r="N48" t="s">
         <v>119</v>
       </c>
-      <c r="O48" s="6">
+      <c r="O48" s="5">
         <f>IF(P48&lt;&gt;"", VLOOKUP(P48, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -19463,7 +19463,7 @@
       <c r="M49" t="s">
         <v>50</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O49" s="5">
         <f>IF(P49&lt;&gt;"", VLOOKUP(P49, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19529,7 +19529,7 @@
       <c r="M50" t="s">
         <v>50</v>
       </c>
-      <c r="O50" s="6">
+      <c r="O50" s="5">
         <f>IF(P50&lt;&gt;"", VLOOKUP(P50, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19598,7 +19598,7 @@
       <c r="N51" t="s">
         <v>28</v>
       </c>
-      <c r="O51" s="6">
+      <c r="O51" s="5">
         <f>IF(P51&lt;&gt;"", VLOOKUP(P51, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -19667,7 +19667,7 @@
       <c r="M52" t="s">
         <v>50</v>
       </c>
-      <c r="O52" s="6">
+      <c r="O52" s="5">
         <f>IF(P52&lt;&gt;"", VLOOKUP(P52, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19736,7 +19736,7 @@
       <c r="N53" t="s">
         <v>28</v>
       </c>
-      <c r="O53" s="6">
+      <c r="O53" s="5">
         <f>IF(P53&lt;&gt;"", VLOOKUP(P53, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -19805,7 +19805,7 @@
       <c r="M54" t="s">
         <v>50</v>
       </c>
-      <c r="O54" s="6">
+      <c r="O54" s="5">
         <f>IF(P54&lt;&gt;"", VLOOKUP(P54, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19865,7 +19865,7 @@
       <c r="M55" t="s">
         <v>50</v>
       </c>
-      <c r="O55" s="6">
+      <c r="O55" s="5">
         <f>IF(P55&lt;&gt;"", VLOOKUP(P55, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19931,7 +19931,7 @@
       <c r="M56" t="s">
         <v>50</v>
       </c>
-      <c r="O56" s="6">
+      <c r="O56" s="5">
         <f>IF(P56&lt;&gt;"", VLOOKUP(P56, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -19997,7 +19997,7 @@
       <c r="M57" t="s">
         <v>50</v>
       </c>
-      <c r="O57" s="6">
+      <c r="O57" s="5">
         <f>IF(P57&lt;&gt;"", VLOOKUP(P57, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20057,7 +20057,7 @@
       <c r="M58" t="s">
         <v>50</v>
       </c>
-      <c r="O58" s="6">
+      <c r="O58" s="5">
         <f>IF(P58&lt;&gt;"", VLOOKUP(P58, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="N59" t="s">
         <v>28</v>
       </c>
-      <c r="O59" s="6">
+      <c r="O59" s="5">
         <f>IF(P59&lt;&gt;"", VLOOKUP(P59, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -20195,7 +20195,7 @@
       <c r="M60" t="s">
         <v>50</v>
       </c>
-      <c r="O60" s="6">
+      <c r="O60" s="5">
         <f>IF(P60&lt;&gt;"", VLOOKUP(P60, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20261,7 +20261,7 @@
       <c r="M61" t="s">
         <v>50</v>
       </c>
-      <c r="O61" s="6">
+      <c r="O61" s="5">
         <f>IF(P61&lt;&gt;"", VLOOKUP(P61, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20327,7 +20327,7 @@
       <c r="M62" t="s">
         <v>50</v>
       </c>
-      <c r="O62" s="6">
+      <c r="O62" s="5">
         <f>IF(P62&lt;&gt;"", VLOOKUP(P62, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20396,7 +20396,7 @@
       <c r="N63" t="s">
         <v>28</v>
       </c>
-      <c r="O63" s="6">
+      <c r="O63" s="5">
         <f>IF(P63&lt;&gt;"", VLOOKUP(P63, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -20459,7 +20459,7 @@
       <c r="M64" t="s">
         <v>50</v>
       </c>
-      <c r="O64" s="6">
+      <c r="O64" s="5">
         <f>IF(P64&lt;&gt;"", VLOOKUP(P64, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20519,7 +20519,7 @@
       <c r="M65" t="s">
         <v>50</v>
       </c>
-      <c r="O65" s="6">
+      <c r="O65" s="5">
         <f>IF(P65&lt;&gt;"", VLOOKUP(P65, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20588,7 +20588,7 @@
       <c r="M66" t="s">
         <v>50</v>
       </c>
-      <c r="O66" s="6">
+      <c r="O66" s="5">
         <f>IF(P66&lt;&gt;"", VLOOKUP(P66, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20657,7 +20657,7 @@
       <c r="N67" t="s">
         <v>28</v>
       </c>
-      <c r="O67" s="6">
+      <c r="O67" s="5">
         <f>IF(P67&lt;&gt;"", VLOOKUP(P67, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -20729,7 +20729,7 @@
       <c r="N68" t="s">
         <v>28</v>
       </c>
-      <c r="O68" s="6">
+      <c r="O68" s="5">
         <f>IF(P68&lt;&gt;"", VLOOKUP(P68, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -20792,7 +20792,7 @@
       <c r="M69" t="s">
         <v>50</v>
       </c>
-      <c r="O69" s="6">
+      <c r="O69" s="5">
         <f>IF(P69&lt;&gt;"", VLOOKUP(P69, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20858,7 +20858,7 @@
       <c r="M70" t="s">
         <v>50</v>
       </c>
-      <c r="O70" s="6">
+      <c r="O70" s="5">
         <f>IF(P70&lt;&gt;"", VLOOKUP(P70, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20924,7 +20924,7 @@
       <c r="M71" t="s">
         <v>50</v>
       </c>
-      <c r="O71" s="6">
+      <c r="O71" s="5">
         <f>IF(P71&lt;&gt;"", VLOOKUP(P71, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -20993,7 +20993,7 @@
       <c r="N72" t="s">
         <v>119</v>
       </c>
-      <c r="O72" s="6">
+      <c r="O72" s="5">
         <f>IF(P72&lt;&gt;"", VLOOKUP(P72, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -21062,7 +21062,7 @@
       <c r="M73" t="s">
         <v>50</v>
       </c>
-      <c r="O73" s="6">
+      <c r="O73" s="5">
         <f>IF(P73&lt;&gt;"", VLOOKUP(P73, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21122,7 +21122,7 @@
       <c r="M74" t="s">
         <v>25</v>
       </c>
-      <c r="O74" s="6">
+      <c r="O74" s="5">
         <f>IF(P74&lt;&gt;"", VLOOKUP(P74, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -21194,7 +21194,7 @@
       <c r="N75" t="s">
         <v>51</v>
       </c>
-      <c r="O75" s="6">
+      <c r="O75" s="5">
         <f>IF(P75&lt;&gt;"", VLOOKUP(P75, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -21263,7 +21263,7 @@
       <c r="M76" t="s">
         <v>50</v>
       </c>
-      <c r="O76" s="6">
+      <c r="O76" s="5">
         <f>IF(P76&lt;&gt;"", VLOOKUP(P76, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21329,7 +21329,7 @@
       <c r="M77" t="s">
         <v>50</v>
       </c>
-      <c r="O77" s="6">
+      <c r="O77" s="5">
         <f>IF(P77&lt;&gt;"", VLOOKUP(P77, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21398,7 +21398,7 @@
       <c r="N78" t="s">
         <v>28</v>
       </c>
-      <c r="O78" s="6">
+      <c r="O78" s="5">
         <f>IF(P78&lt;&gt;"", VLOOKUP(P78, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -21470,7 +21470,7 @@
       <c r="N79" t="s">
         <v>28</v>
       </c>
-      <c r="O79" s="6">
+      <c r="O79" s="5">
         <f>IF(P79&lt;&gt;"", VLOOKUP(P79, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -21542,7 +21542,7 @@
       <c r="N80" t="s">
         <v>68</v>
       </c>
-      <c r="O80" s="6">
+      <c r="O80" s="5">
         <f>IF(P80&lt;&gt;"", VLOOKUP(P80, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -21605,7 +21605,7 @@
       <c r="M81" t="s">
         <v>50</v>
       </c>
-      <c r="O81" s="6">
+      <c r="O81" s="5">
         <f>IF(P81&lt;&gt;"", VLOOKUP(P81, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21671,7 +21671,7 @@
       <c r="M82" t="s">
         <v>50</v>
       </c>
-      <c r="O82" s="6">
+      <c r="O82" s="5">
         <f>IF(P82&lt;&gt;"", VLOOKUP(P82, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21731,7 +21731,7 @@
       <c r="M83" t="s">
         <v>50</v>
       </c>
-      <c r="O83" s="6">
+      <c r="O83" s="5">
         <f>IF(P83&lt;&gt;"", VLOOKUP(P83, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21791,7 +21791,7 @@
       <c r="M84" t="s">
         <v>25</v>
       </c>
-      <c r="O84" s="6">
+      <c r="O84" s="5">
         <f>IF(P84&lt;&gt;"", VLOOKUP(P84, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -21860,7 +21860,7 @@
       <c r="M85" t="s">
         <v>50</v>
       </c>
-      <c r="O85" s="6">
+      <c r="O85" s="5">
         <f>IF(P85&lt;&gt;"", VLOOKUP(P85, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -21929,7 +21929,7 @@
       <c r="N86" t="s">
         <v>68</v>
       </c>
-      <c r="O86" s="6">
+      <c r="O86" s="5">
         <f>IF(P86&lt;&gt;"", VLOOKUP(P86, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -21998,7 +21998,7 @@
       <c r="M87" t="s">
         <v>50</v>
       </c>
-      <c r="O87" s="6">
+      <c r="O87" s="5">
         <f>IF(P87&lt;&gt;"", VLOOKUP(P87, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22058,7 +22058,7 @@
       <c r="M88" t="s">
         <v>50</v>
       </c>
-      <c r="O88" s="6">
+      <c r="O88" s="5">
         <f>IF(P88&lt;&gt;"", VLOOKUP(P88, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22124,7 +22124,7 @@
       <c r="M89" t="s">
         <v>50</v>
       </c>
-      <c r="O89" s="6">
+      <c r="O89" s="5">
         <f>IF(P89&lt;&gt;"", VLOOKUP(P89, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22184,7 +22184,7 @@
       <c r="M90" t="s">
         <v>50</v>
       </c>
-      <c r="O90" s="6">
+      <c r="O90" s="5">
         <f>IF(P90&lt;&gt;"", VLOOKUP(P90, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22244,7 +22244,7 @@
       <c r="M91" t="s">
         <v>25</v>
       </c>
-      <c r="O91" s="6">
+      <c r="O91" s="5">
         <f>IF(P91&lt;&gt;"", VLOOKUP(P91, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -22307,7 +22307,7 @@
       <c r="M92" t="s">
         <v>50</v>
       </c>
-      <c r="O92" s="6">
+      <c r="O92" s="5">
         <f>IF(P92&lt;&gt;"", VLOOKUP(P92, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22373,7 +22373,7 @@
       <c r="M93" t="s">
         <v>50</v>
       </c>
-      <c r="O93" s="6">
+      <c r="O93" s="5">
         <f>IF(P93&lt;&gt;"", VLOOKUP(P93, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22433,7 +22433,7 @@
       <c r="M94" t="s">
         <v>25</v>
       </c>
-      <c r="O94" s="6">
+      <c r="O94" s="5">
         <f>IF(P94&lt;&gt;"", VLOOKUP(P94, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -22496,7 +22496,7 @@
       <c r="M95" t="s">
         <v>25</v>
       </c>
-      <c r="O95" s="6">
+      <c r="O95" s="5">
         <f>IF(P95&lt;&gt;"", VLOOKUP(P95, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -22568,7 +22568,7 @@
       <c r="N96" t="s">
         <v>68</v>
       </c>
-      <c r="O96" s="6">
+      <c r="O96" s="5">
         <f>IF(P96&lt;&gt;"", VLOOKUP(P96, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -22631,7 +22631,7 @@
       <c r="M97" t="s">
         <v>50</v>
       </c>
-      <c r="O97" s="6">
+      <c r="O97" s="5">
         <f>IF(P97&lt;&gt;"", VLOOKUP(P97, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22700,7 +22700,7 @@
       <c r="N98" t="s">
         <v>28</v>
       </c>
-      <c r="O98" s="6">
+      <c r="O98" s="5">
         <f>IF(P98&lt;&gt;"", VLOOKUP(P98, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -22763,7 +22763,7 @@
       <c r="M99" t="s">
         <v>50</v>
       </c>
-      <c r="O99" s="6">
+      <c r="O99" s="5">
         <f>IF(P99&lt;&gt;"", VLOOKUP(P99, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22823,7 +22823,7 @@
       <c r="M100" t="s">
         <v>50</v>
       </c>
-      <c r="O100" s="6">
+      <c r="O100" s="5">
         <f>IF(P100&lt;&gt;"", VLOOKUP(P100, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -22892,7 +22892,7 @@
       <c r="N101" t="s">
         <v>28</v>
       </c>
-      <c r="O101" s="6">
+      <c r="O101" s="5">
         <f>IF(P101&lt;&gt;"", VLOOKUP(P101, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -22961,7 +22961,7 @@
       <c r="M102" t="s">
         <v>50</v>
       </c>
-      <c r="O102" s="6">
+      <c r="O102" s="5">
         <f>IF(P102&lt;&gt;"", VLOOKUP(P102, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23027,7 +23027,7 @@
       <c r="M103" t="s">
         <v>50</v>
       </c>
-      <c r="O103" s="6">
+      <c r="O103" s="5">
         <f>IF(P103&lt;&gt;"", VLOOKUP(P103, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23087,7 +23087,7 @@
       <c r="M104" t="s">
         <v>50</v>
       </c>
-      <c r="O104" s="6">
+      <c r="O104" s="5">
         <f>IF(P104&lt;&gt;"", VLOOKUP(P104, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23156,7 +23156,7 @@
       <c r="N105" t="s">
         <v>28</v>
       </c>
-      <c r="O105" s="6">
+      <c r="O105" s="5">
         <f>IF(P105&lt;&gt;"", VLOOKUP(P105, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -23219,7 +23219,7 @@
       <c r="M106" t="s">
         <v>25</v>
       </c>
-      <c r="O106" s="6">
+      <c r="O106" s="5">
         <f>IF(P106&lt;&gt;"", VLOOKUP(P106, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -23282,7 +23282,7 @@
       <c r="M107" t="s">
         <v>25</v>
       </c>
-      <c r="O107" s="6">
+      <c r="O107" s="5">
         <f>IF(P107&lt;&gt;"", VLOOKUP(P107, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -23354,7 +23354,7 @@
       <c r="N108" t="s">
         <v>28</v>
       </c>
-      <c r="O108" s="6">
+      <c r="O108" s="5">
         <f>IF(P108&lt;&gt;"", VLOOKUP(P108, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -23423,7 +23423,7 @@
       <c r="M109" t="s">
         <v>50</v>
       </c>
-      <c r="O109" s="6">
+      <c r="O109" s="5">
         <f>IF(P109&lt;&gt;"", VLOOKUP(P109, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23489,7 +23489,7 @@
       <c r="M110" t="s">
         <v>50</v>
       </c>
-      <c r="O110" s="6">
+      <c r="O110" s="5">
         <f>IF(P110&lt;&gt;"", VLOOKUP(P110, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23555,7 +23555,7 @@
       <c r="M111" t="s">
         <v>50</v>
       </c>
-      <c r="O111" s="6">
+      <c r="O111" s="5">
         <f>IF(P111&lt;&gt;"", VLOOKUP(P111, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23621,7 +23621,7 @@
       <c r="M112" t="s">
         <v>50</v>
       </c>
-      <c r="O112" s="6">
+      <c r="O112" s="5">
         <f>IF(P112&lt;&gt;"", VLOOKUP(P112, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23690,7 +23690,7 @@
       <c r="N113" t="s">
         <v>28</v>
       </c>
-      <c r="O113" s="6">
+      <c r="O113" s="5">
         <f>IF(P113&lt;&gt;"", VLOOKUP(P113, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -23759,7 +23759,7 @@
       <c r="M114" t="s">
         <v>50</v>
       </c>
-      <c r="O114" s="6">
+      <c r="O114" s="5">
         <f>IF(P114&lt;&gt;"", VLOOKUP(P114, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23825,7 +23825,7 @@
       <c r="M115" t="s">
         <v>50</v>
       </c>
-      <c r="O115" s="6">
+      <c r="O115" s="5">
         <f>IF(P115&lt;&gt;"", VLOOKUP(P115, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23891,7 +23891,7 @@
       <c r="M116" t="s">
         <v>50</v>
       </c>
-      <c r="O116" s="6">
+      <c r="O116" s="5">
         <f>IF(P116&lt;&gt;"", VLOOKUP(P116, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -23960,7 +23960,7 @@
       <c r="N117" t="s">
         <v>68</v>
       </c>
-      <c r="O117" s="6">
+      <c r="O117" s="5">
         <f>IF(P117&lt;&gt;"", VLOOKUP(P117, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -24029,7 +24029,7 @@
       <c r="M118" t="s">
         <v>50</v>
       </c>
-      <c r="O118" s="6">
+      <c r="O118" s="5">
         <f>IF(P118&lt;&gt;"", VLOOKUP(P118, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24098,7 +24098,7 @@
       <c r="N119" t="s">
         <v>28</v>
       </c>
-      <c r="O119" s="6">
+      <c r="O119" s="5">
         <f>IF(P119&lt;&gt;"", VLOOKUP(P119, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -24161,7 +24161,7 @@
       <c r="M120" t="s">
         <v>25</v>
       </c>
-      <c r="O120" s="6">
+      <c r="O120" s="5">
         <f>IF(P120&lt;&gt;"", VLOOKUP(P120, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -24233,7 +24233,7 @@
       <c r="N121" t="s">
         <v>119</v>
       </c>
-      <c r="O121" s="6">
+      <c r="O121" s="5">
         <f>IF(P121&lt;&gt;"", VLOOKUP(P121, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -24302,7 +24302,7 @@
       <c r="M122" t="s">
         <v>50</v>
       </c>
-      <c r="O122" s="6">
+      <c r="O122" s="5">
         <f>IF(P122&lt;&gt;"", VLOOKUP(P122, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24362,7 +24362,7 @@
       <c r="M123" t="s">
         <v>25</v>
       </c>
-      <c r="O123" s="6">
+      <c r="O123" s="5">
         <f>IF(P123&lt;&gt;"", VLOOKUP(P123, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -24434,7 +24434,7 @@
       <c r="N124" t="s">
         <v>28</v>
       </c>
-      <c r="O124" s="6">
+      <c r="O124" s="5">
         <f>IF(P124&lt;&gt;"", VLOOKUP(P124, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -24503,7 +24503,7 @@
       <c r="M125" t="s">
         <v>50</v>
       </c>
-      <c r="O125" s="6">
+      <c r="O125" s="5">
         <f>IF(P125&lt;&gt;"", VLOOKUP(P125, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24575,7 +24575,7 @@
       <c r="N126" t="s">
         <v>119</v>
       </c>
-      <c r="O126" s="6">
+      <c r="O126" s="5">
         <f>IF(P126&lt;&gt;"", VLOOKUP(P126, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -24647,7 +24647,7 @@
       <c r="N127" t="s">
         <v>68</v>
       </c>
-      <c r="O127" s="6">
+      <c r="O127" s="5">
         <f>IF(P127&lt;&gt;"", VLOOKUP(P127, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -24716,7 +24716,7 @@
       <c r="M128" t="s">
         <v>50</v>
       </c>
-      <c r="O128" s="6">
+      <c r="O128" s="5">
         <f>IF(P128&lt;&gt;"", VLOOKUP(P128, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24776,7 +24776,7 @@
       <c r="M129" t="s">
         <v>50</v>
       </c>
-      <c r="O129" s="6">
+      <c r="O129" s="5">
         <f>IF(P129&lt;&gt;"", VLOOKUP(P129, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24836,7 +24836,7 @@
       <c r="M130" t="s">
         <v>50</v>
       </c>
-      <c r="O130" s="6">
+      <c r="O130" s="5">
         <f>IF(P130&lt;&gt;"", VLOOKUP(P130, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24896,7 +24896,7 @@
       <c r="M131" t="s">
         <v>50</v>
       </c>
-      <c r="O131" s="6">
+      <c r="O131" s="5">
         <f>IF(P131&lt;&gt;"", VLOOKUP(P131, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -24962,7 +24962,7 @@
       <c r="M132" t="s">
         <v>50</v>
       </c>
-      <c r="O132" s="6">
+      <c r="O132" s="5">
         <f>IF(P132&lt;&gt;"", VLOOKUP(P132, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25031,7 +25031,7 @@
       <c r="N133" t="s">
         <v>68</v>
       </c>
-      <c r="O133" s="6">
+      <c r="O133" s="5">
         <f>IF(P133&lt;&gt;"", VLOOKUP(P133, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -25103,7 +25103,7 @@
       <c r="N134" t="s">
         <v>28</v>
       </c>
-      <c r="O134" s="6">
+      <c r="O134" s="5">
         <f>IF(P134&lt;&gt;"", VLOOKUP(P134, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -25175,7 +25175,7 @@
       <c r="N135" t="s">
         <v>28</v>
       </c>
-      <c r="O135" s="6">
+      <c r="O135" s="5">
         <f>IF(P135&lt;&gt;"", VLOOKUP(P135, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -25244,7 +25244,7 @@
       <c r="M136" t="s">
         <v>50</v>
       </c>
-      <c r="O136" s="6">
+      <c r="O136" s="5">
         <f>IF(P136&lt;&gt;"", VLOOKUP(P136, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25304,7 +25304,7 @@
       <c r="M137" t="s">
         <v>25</v>
       </c>
-      <c r="O137" s="6">
+      <c r="O137" s="5">
         <f>IF(P137&lt;&gt;"", VLOOKUP(P137, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -25373,7 +25373,7 @@
       <c r="M138" t="s">
         <v>50</v>
       </c>
-      <c r="O138" s="6">
+      <c r="O138" s="5">
         <f>IF(P138&lt;&gt;"", VLOOKUP(P138, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25439,7 +25439,7 @@
       <c r="M139" t="s">
         <v>50</v>
       </c>
-      <c r="O139" s="6">
+      <c r="O139" s="5">
         <f>IF(P139&lt;&gt;"", VLOOKUP(P139, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25505,7 +25505,7 @@
       <c r="M140" t="s">
         <v>50</v>
       </c>
-      <c r="O140" s="6">
+      <c r="O140" s="5">
         <f>IF(P140&lt;&gt;"", VLOOKUP(P140, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25565,7 +25565,7 @@
       <c r="M141" t="s">
         <v>50</v>
       </c>
-      <c r="O141" s="6">
+      <c r="O141" s="5">
         <f>IF(P141&lt;&gt;"", VLOOKUP(P141, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25625,7 +25625,7 @@
       <c r="M142" t="s">
         <v>50</v>
       </c>
-      <c r="O142" s="6">
+      <c r="O142" s="5">
         <f>IF(P142&lt;&gt;"", VLOOKUP(P142, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25691,7 +25691,7 @@
       <c r="M143" t="s">
         <v>50</v>
       </c>
-      <c r="O143" s="6">
+      <c r="O143" s="5">
         <f>IF(P143&lt;&gt;"", VLOOKUP(P143, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25757,7 +25757,7 @@
       <c r="M144" t="s">
         <v>50</v>
       </c>
-      <c r="O144" s="6">
+      <c r="O144" s="5">
         <f>IF(P144&lt;&gt;"", VLOOKUP(P144, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25826,7 +25826,7 @@
       <c r="N145" t="s">
         <v>28</v>
       </c>
-      <c r="O145" s="6">
+      <c r="O145" s="5">
         <f>IF(P145&lt;&gt;"", VLOOKUP(P145, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -25895,7 +25895,7 @@
       <c r="M146" t="s">
         <v>50</v>
       </c>
-      <c r="O146" s="6">
+      <c r="O146" s="5">
         <f>IF(P146&lt;&gt;"", VLOOKUP(P146, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -25961,7 +25961,7 @@
       <c r="M147" t="s">
         <v>50</v>
       </c>
-      <c r="O147" s="6">
+      <c r="O147" s="5">
         <f>IF(P147&lt;&gt;"", VLOOKUP(P147, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26021,7 +26021,7 @@
       <c r="M148" t="s">
         <v>50</v>
       </c>
-      <c r="O148" s="6">
+      <c r="O148" s="5">
         <f>IF(P148&lt;&gt;"", VLOOKUP(P148, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26081,7 +26081,7 @@
       <c r="M149" t="s">
         <v>50</v>
       </c>
-      <c r="O149" s="6">
+      <c r="O149" s="5">
         <f>IF(P149&lt;&gt;"", VLOOKUP(P149, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26141,7 +26141,7 @@
       <c r="M150" t="s">
         <v>25</v>
       </c>
-      <c r="O150" s="6">
+      <c r="O150" s="5">
         <f>IF(P150&lt;&gt;"", VLOOKUP(P150, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -26204,7 +26204,7 @@
       <c r="M151" t="s">
         <v>25</v>
       </c>
-      <c r="O151" s="6">
+      <c r="O151" s="5">
         <f>IF(P151&lt;&gt;"", VLOOKUP(P151, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -26273,7 +26273,7 @@
       <c r="M152" t="s">
         <v>50</v>
       </c>
-      <c r="O152" s="6">
+      <c r="O152" s="5">
         <f>IF(P152&lt;&gt;"", VLOOKUP(P152, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26339,7 +26339,7 @@
       <c r="M153" t="s">
         <v>50</v>
       </c>
-      <c r="O153" s="6">
+      <c r="O153" s="5">
         <f>IF(P153&lt;&gt;"", VLOOKUP(P153, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26405,7 +26405,7 @@
       <c r="M154" t="s">
         <v>50</v>
       </c>
-      <c r="O154" s="6">
+      <c r="O154" s="5">
         <f>IF(P154&lt;&gt;"", VLOOKUP(P154, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26471,7 +26471,7 @@
       <c r="M155" t="s">
         <v>50</v>
       </c>
-      <c r="O155" s="6">
+      <c r="O155" s="5">
         <f>IF(P155&lt;&gt;"", VLOOKUP(P155, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26531,7 +26531,7 @@
       <c r="M156" t="s">
         <v>50</v>
       </c>
-      <c r="O156" s="6">
+      <c r="O156" s="5">
         <f>IF(P156&lt;&gt;"", VLOOKUP(P156, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26591,7 +26591,7 @@
       <c r="M157" t="s">
         <v>25</v>
       </c>
-      <c r="O157" s="6">
+      <c r="O157" s="5">
         <f>IF(P157&lt;&gt;"", VLOOKUP(P157, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -26663,7 +26663,7 @@
       <c r="N158" t="s">
         <v>28</v>
       </c>
-      <c r="O158" s="6">
+      <c r="O158" s="5">
         <f>IF(P158&lt;&gt;"", VLOOKUP(P158, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -26735,7 +26735,7 @@
       <c r="N159" t="s">
         <v>68</v>
       </c>
-      <c r="O159" s="6">
+      <c r="O159" s="5">
         <f>IF(P159&lt;&gt;"", VLOOKUP(P159, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -26804,7 +26804,7 @@
       <c r="M160" t="s">
         <v>50</v>
       </c>
-      <c r="O160" s="6">
+      <c r="O160" s="5">
         <f>IF(P160&lt;&gt;"", VLOOKUP(P160, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26870,7 +26870,7 @@
       <c r="M161" t="s">
         <v>50</v>
       </c>
-      <c r="O161" s="6">
+      <c r="O161" s="5">
         <f>IF(P161&lt;&gt;"", VLOOKUP(P161, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -26939,7 +26939,7 @@
       <c r="N162" t="s">
         <v>119</v>
       </c>
-      <c r="O162" s="6">
+      <c r="O162" s="5">
         <f>IF(P162&lt;&gt;"", VLOOKUP(P162, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -27008,7 +27008,7 @@
       <c r="M163" t="s">
         <v>50</v>
       </c>
-      <c r="O163" s="6">
+      <c r="O163" s="5">
         <f>IF(P163&lt;&gt;"", VLOOKUP(P163, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27068,7 +27068,7 @@
       <c r="M164" t="s">
         <v>50</v>
       </c>
-      <c r="O164" s="6">
+      <c r="O164" s="5">
         <f>IF(P164&lt;&gt;"", VLOOKUP(P164, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27134,7 +27134,7 @@
       <c r="M165" t="s">
         <v>50</v>
       </c>
-      <c r="O165" s="6">
+      <c r="O165" s="5">
         <f>IF(P165&lt;&gt;"", VLOOKUP(P165, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27194,7 +27194,7 @@
       <c r="M166" t="s">
         <v>50</v>
       </c>
-      <c r="O166" s="6">
+      <c r="O166" s="5">
         <f>IF(P166&lt;&gt;"", VLOOKUP(P166, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27263,7 +27263,7 @@
       <c r="N167" t="s">
         <v>119</v>
       </c>
-      <c r="O167" s="6">
+      <c r="O167" s="5">
         <f>IF(P167&lt;&gt;"", VLOOKUP(P167, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -27335,7 +27335,7 @@
       <c r="N168" t="s">
         <v>28</v>
       </c>
-      <c r="O168" s="6">
+      <c r="O168" s="5">
         <f>IF(P168&lt;&gt;"", VLOOKUP(P168, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -27404,7 +27404,7 @@
       <c r="M169" t="s">
         <v>50</v>
       </c>
-      <c r="O169" s="6">
+      <c r="O169" s="5">
         <f>IF(P169&lt;&gt;"", VLOOKUP(P169, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27464,7 +27464,7 @@
       <c r="M170" t="s">
         <v>50</v>
       </c>
-      <c r="O170" s="6">
+      <c r="O170" s="5">
         <f>IF(P170&lt;&gt;"", VLOOKUP(P170, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27533,7 +27533,7 @@
       <c r="N171" t="s">
         <v>28</v>
       </c>
-      <c r="O171" s="6">
+      <c r="O171" s="5">
         <f>IF(P171&lt;&gt;"", VLOOKUP(P171, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -27602,7 +27602,7 @@
       <c r="M172" t="s">
         <v>50</v>
       </c>
-      <c r="O172" s="6">
+      <c r="O172" s="5">
         <f>IF(P172&lt;&gt;"", VLOOKUP(P172, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27668,7 +27668,7 @@
       <c r="M173" t="s">
         <v>50</v>
       </c>
-      <c r="O173" s="6">
+      <c r="O173" s="5">
         <f>IF(P173&lt;&gt;"", VLOOKUP(P173, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27737,7 +27737,7 @@
       <c r="N174" t="s">
         <v>28</v>
       </c>
-      <c r="O174" s="6">
+      <c r="O174" s="5">
         <f>IF(P174&lt;&gt;"", VLOOKUP(P174, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -27800,7 +27800,7 @@
       <c r="M175" t="s">
         <v>50</v>
       </c>
-      <c r="O175" s="6">
+      <c r="O175" s="5">
         <f>IF(P175&lt;&gt;"", VLOOKUP(P175, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27860,7 +27860,7 @@
       <c r="M176" t="s">
         <v>50</v>
       </c>
-      <c r="O176" s="6">
+      <c r="O176" s="5">
         <f>IF(P176&lt;&gt;"", VLOOKUP(P176, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27920,7 +27920,7 @@
       <c r="M177" t="s">
         <v>50</v>
       </c>
-      <c r="O177" s="6">
+      <c r="O177" s="5">
         <f>IF(P177&lt;&gt;"", VLOOKUP(P177, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -27989,7 +27989,7 @@
       <c r="M178" t="s">
         <v>50</v>
       </c>
-      <c r="O178" s="6">
+      <c r="O178" s="5">
         <f>IF(P178&lt;&gt;"", VLOOKUP(P178, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28055,7 +28055,7 @@
       <c r="M179" t="s">
         <v>50</v>
       </c>
-      <c r="O179" s="6">
+      <c r="O179" s="5">
         <f>IF(P179&lt;&gt;"", VLOOKUP(P179, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28115,7 +28115,7 @@
       <c r="M180" t="s">
         <v>50</v>
       </c>
-      <c r="O180" s="6">
+      <c r="O180" s="5">
         <f>IF(P180&lt;&gt;"", VLOOKUP(P180, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28175,7 +28175,7 @@
       <c r="M181" t="s">
         <v>25</v>
       </c>
-      <c r="O181" s="6">
+      <c r="O181" s="5">
         <f>IF(P181&lt;&gt;"", VLOOKUP(P181, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -28247,7 +28247,7 @@
       <c r="N182" t="s">
         <v>28</v>
       </c>
-      <c r="O182" s="6">
+      <c r="O182" s="5">
         <f>IF(P182&lt;&gt;"", VLOOKUP(P182, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -28310,7 +28310,7 @@
       <c r="M183" t="s">
         <v>50</v>
       </c>
-      <c r="O183" s="6">
+      <c r="O183" s="5">
         <f>IF(P183&lt;&gt;"", VLOOKUP(P183, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28379,7 +28379,7 @@
       <c r="N184" t="s">
         <v>28</v>
       </c>
-      <c r="O184" s="6">
+      <c r="O184" s="5">
         <f>IF(P184&lt;&gt;"", VLOOKUP(P184, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -28448,7 +28448,7 @@
       <c r="M185" t="s">
         <v>50</v>
       </c>
-      <c r="O185" s="6">
+      <c r="O185" s="5">
         <f>IF(P185&lt;&gt;"", VLOOKUP(P185, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28508,7 +28508,7 @@
       <c r="M186" t="s">
         <v>50</v>
       </c>
-      <c r="O186" s="6">
+      <c r="O186" s="5">
         <f>IF(P186&lt;&gt;"", VLOOKUP(P186, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28577,7 +28577,7 @@
       <c r="N187" t="s">
         <v>68</v>
       </c>
-      <c r="O187" s="6">
+      <c r="O187" s="5">
         <f>IF(P187&lt;&gt;"", VLOOKUP(P187, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -28640,7 +28640,7 @@
       <c r="M188" t="s">
         <v>50</v>
       </c>
-      <c r="O188" s="6">
+      <c r="O188" s="5">
         <f>IF(P188&lt;&gt;"", VLOOKUP(P188, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28706,7 +28706,7 @@
       <c r="M189" t="s">
         <v>50</v>
       </c>
-      <c r="O189" s="6">
+      <c r="O189" s="5">
         <f>IF(P189&lt;&gt;"", VLOOKUP(P189, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28775,7 +28775,7 @@
       <c r="N190" t="s">
         <v>28</v>
       </c>
-      <c r="O190" s="6">
+      <c r="O190" s="5">
         <f>IF(P190&lt;&gt;"", VLOOKUP(P190, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -28844,7 +28844,7 @@
       <c r="M191" t="s">
         <v>50</v>
       </c>
-      <c r="O191" s="6">
+      <c r="O191" s="5">
         <f>IF(P191&lt;&gt;"", VLOOKUP(P191, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -28913,7 +28913,7 @@
       <c r="N192" t="s">
         <v>28</v>
       </c>
-      <c r="O192" s="6">
+      <c r="O192" s="5">
         <f>IF(P192&lt;&gt;"", VLOOKUP(P192, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -28982,7 +28982,7 @@
       <c r="M193" t="s">
         <v>50</v>
       </c>
-      <c r="O193" s="6">
+      <c r="O193" s="5">
         <f>IF(P193&lt;&gt;"", VLOOKUP(P193, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29048,7 +29048,7 @@
       <c r="M194" t="s">
         <v>50</v>
       </c>
-      <c r="O194" s="6">
+      <c r="O194" s="5">
         <f>IF(P194&lt;&gt;"", VLOOKUP(P194, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29114,7 +29114,7 @@
       <c r="M195" t="s">
         <v>50</v>
       </c>
-      <c r="O195" s="6">
+      <c r="O195" s="5">
         <f>IF(P195&lt;&gt;"", VLOOKUP(P195, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29180,7 +29180,7 @@
       <c r="M196" t="s">
         <v>50</v>
       </c>
-      <c r="O196" s="6">
+      <c r="O196" s="5">
         <f>IF(P196&lt;&gt;"", VLOOKUP(P196, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29246,7 +29246,7 @@
       <c r="M197" t="s">
         <v>50</v>
       </c>
-      <c r="O197" s="6">
+      <c r="O197" s="5">
         <f>IF(P197&lt;&gt;"", VLOOKUP(P197, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29315,7 +29315,7 @@
       <c r="N198" t="s">
         <v>68</v>
       </c>
-      <c r="O198" s="6">
+      <c r="O198" s="5">
         <f>IF(P198&lt;&gt;"", VLOOKUP(P198, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -29387,7 +29387,7 @@
       <c r="N199" t="s">
         <v>28</v>
       </c>
-      <c r="O199" s="6">
+      <c r="O199" s="5">
         <f>IF(P199&lt;&gt;"", VLOOKUP(P199, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -29459,7 +29459,7 @@
       <c r="N200" t="s">
         <v>68</v>
       </c>
-      <c r="O200" s="6">
+      <c r="O200" s="5">
         <f>IF(P200&lt;&gt;"", VLOOKUP(P200, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -29528,7 +29528,7 @@
       <c r="M201" t="s">
         <v>50</v>
       </c>
-      <c r="O201" s="6">
+      <c r="O201" s="5">
         <f>IF(P201&lt;&gt;"", VLOOKUP(P201, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29588,7 +29588,7 @@
       <c r="M202" t="s">
         <v>50</v>
       </c>
-      <c r="O202" s="6">
+      <c r="O202" s="5">
         <f>IF(P202&lt;&gt;"", VLOOKUP(P202, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29648,7 +29648,7 @@
       <c r="M203" t="s">
         <v>25</v>
       </c>
-      <c r="O203" s="6">
+      <c r="O203" s="5">
         <f>IF(P203&lt;&gt;"", VLOOKUP(P203, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -29717,7 +29717,7 @@
       <c r="M204" t="s">
         <v>50</v>
       </c>
-      <c r="O204" s="6">
+      <c r="O204" s="5">
         <f>IF(P204&lt;&gt;"", VLOOKUP(P204, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29777,7 +29777,7 @@
       <c r="M205" t="s">
         <v>50</v>
       </c>
-      <c r="O205" s="6">
+      <c r="O205" s="5">
         <f>IF(P205&lt;&gt;"", VLOOKUP(P205, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29843,7 +29843,7 @@
       <c r="M206" t="s">
         <v>50</v>
       </c>
-      <c r="O206" s="6">
+      <c r="O206" s="5">
         <f>IF(P206&lt;&gt;"", VLOOKUP(P206, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -29912,7 +29912,7 @@
       <c r="N207" t="s">
         <v>28</v>
       </c>
-      <c r="O207" s="6">
+      <c r="O207" s="5">
         <f>IF(P207&lt;&gt;"", VLOOKUP(P207, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -29984,7 +29984,7 @@
       <c r="N208" t="s">
         <v>51</v>
       </c>
-      <c r="O208" s="6">
+      <c r="O208" s="5">
         <f>IF(P208&lt;&gt;"", VLOOKUP(P208, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -30056,7 +30056,7 @@
       <c r="N209" t="s">
         <v>68</v>
       </c>
-      <c r="O209" s="6">
+      <c r="O209" s="5">
         <f>IF(P209&lt;&gt;"", VLOOKUP(P209, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -30125,7 +30125,7 @@
       <c r="M210" t="s">
         <v>50</v>
       </c>
-      <c r="O210" s="6">
+      <c r="O210" s="5">
         <f>IF(P210&lt;&gt;"", VLOOKUP(P210, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30194,7 +30194,7 @@
       <c r="N211" t="s">
         <v>28</v>
       </c>
-      <c r="O211" s="6">
+      <c r="O211" s="5">
         <f>IF(P211&lt;&gt;"", VLOOKUP(P211, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -30266,7 +30266,7 @@
       <c r="N212" t="s">
         <v>119</v>
       </c>
-      <c r="O212" s="6">
+      <c r="O212" s="5">
         <f>IF(P212&lt;&gt;"", VLOOKUP(P212, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -30338,7 +30338,7 @@
       <c r="N213" t="s">
         <v>28</v>
       </c>
-      <c r="O213" s="6">
+      <c r="O213" s="5">
         <f>IF(P213&lt;&gt;"", VLOOKUP(P213, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -30410,7 +30410,7 @@
       <c r="N214" t="s">
         <v>28</v>
       </c>
-      <c r="O214" s="6">
+      <c r="O214" s="5">
         <f>IF(P214&lt;&gt;"", VLOOKUP(P214, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -30479,7 +30479,7 @@
       <c r="M215" t="s">
         <v>50</v>
       </c>
-      <c r="O215" s="6">
+      <c r="O215" s="5">
         <f>IF(P215&lt;&gt;"", VLOOKUP(P215, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30545,7 +30545,7 @@
       <c r="M216" t="s">
         <v>50</v>
       </c>
-      <c r="O216" s="6">
+      <c r="O216" s="5">
         <f>IF(P216&lt;&gt;"", VLOOKUP(P216, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30611,7 +30611,7 @@
       <c r="M217" t="s">
         <v>50</v>
       </c>
-      <c r="O217" s="6">
+      <c r="O217" s="5">
         <f>IF(P217&lt;&gt;"", VLOOKUP(P217, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30671,7 +30671,7 @@
       <c r="M218" t="s">
         <v>50</v>
       </c>
-      <c r="O218" s="6">
+      <c r="O218" s="5">
         <f>IF(P218&lt;&gt;"", VLOOKUP(P218, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30740,7 +30740,7 @@
       <c r="N219" t="s">
         <v>68</v>
       </c>
-      <c r="O219" s="6">
+      <c r="O219" s="5">
         <f>IF(P219&lt;&gt;"", VLOOKUP(P219, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -30809,7 +30809,7 @@
       <c r="M220" t="s">
         <v>50</v>
       </c>
-      <c r="O220" s="6">
+      <c r="O220" s="5">
         <f>IF(P220&lt;&gt;"", VLOOKUP(P220, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30875,7 +30875,7 @@
       <c r="M221" t="s">
         <v>50</v>
       </c>
-      <c r="O221" s="6">
+      <c r="O221" s="5">
         <f>IF(P221&lt;&gt;"", VLOOKUP(P221, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -30941,7 +30941,7 @@
       <c r="M222" t="s">
         <v>50</v>
       </c>
-      <c r="O222" s="6">
+      <c r="O222" s="5">
         <f>IF(P222&lt;&gt;"", VLOOKUP(P222, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31007,7 +31007,7 @@
       <c r="M223" t="s">
         <v>50</v>
       </c>
-      <c r="O223" s="6">
+      <c r="O223" s="5">
         <f>IF(P223&lt;&gt;"", VLOOKUP(P223, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31076,7 +31076,7 @@
       <c r="N224" t="s">
         <v>28</v>
       </c>
-      <c r="O224" s="6">
+      <c r="O224" s="5">
         <f>IF(P224&lt;&gt;"", VLOOKUP(P224, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31145,7 +31145,7 @@
       <c r="M225" t="s">
         <v>50</v>
       </c>
-      <c r="O225" s="6">
+      <c r="O225" s="5">
         <f>IF(P225&lt;&gt;"", VLOOKUP(P225, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31211,7 +31211,7 @@
       <c r="M226" t="s">
         <v>50</v>
       </c>
-      <c r="O226" s="6">
+      <c r="O226" s="5">
         <f>IF(P226&lt;&gt;"", VLOOKUP(P226, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31277,7 +31277,7 @@
       <c r="M227" t="s">
         <v>50</v>
       </c>
-      <c r="O227" s="6">
+      <c r="O227" s="5">
         <f>IF(P227&lt;&gt;"", VLOOKUP(P227, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31343,7 +31343,7 @@
       <c r="M228" t="s">
         <v>50</v>
       </c>
-      <c r="O228" s="6">
+      <c r="O228" s="5">
         <f>IF(P228&lt;&gt;"", VLOOKUP(P228, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31412,7 +31412,7 @@
       <c r="N229" t="s">
         <v>68</v>
       </c>
-      <c r="O229" s="6">
+      <c r="O229" s="5">
         <f>IF(P229&lt;&gt;"", VLOOKUP(P229, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31475,7 +31475,7 @@
       <c r="M230" t="s">
         <v>25</v>
       </c>
-      <c r="O230" s="6">
+      <c r="O230" s="5">
         <f>IF(P230&lt;&gt;"", VLOOKUP(P230, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31547,7 +31547,7 @@
       <c r="N231" t="s">
         <v>51</v>
       </c>
-      <c r="O231" s="6">
+      <c r="O231" s="5">
         <f>IF(P231&lt;&gt;"", VLOOKUP(P231, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31619,7 +31619,7 @@
       <c r="N232" t="s">
         <v>119</v>
       </c>
-      <c r="O232" s="6">
+      <c r="O232" s="5">
         <f>IF(P232&lt;&gt;"", VLOOKUP(P232, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -31691,7 +31691,7 @@
       <c r="N233" t="s">
         <v>68</v>
       </c>
-      <c r="O233" s="6">
+      <c r="O233" s="5">
         <f>IF(P233&lt;&gt;"", VLOOKUP(P233, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31760,7 +31760,7 @@
       <c r="M234" t="s">
         <v>50</v>
       </c>
-      <c r="O234" s="6">
+      <c r="O234" s="5">
         <f>IF(P234&lt;&gt;"", VLOOKUP(P234, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31820,7 +31820,7 @@
       <c r="M235" t="s">
         <v>50</v>
       </c>
-      <c r="O235" s="6">
+      <c r="O235" s="5">
         <f>IF(P235&lt;&gt;"", VLOOKUP(P235, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -31880,7 +31880,7 @@
       <c r="M236" t="s">
         <v>25</v>
       </c>
-      <c r="O236" s="6">
+      <c r="O236" s="5">
         <f>IF(P236&lt;&gt;"", VLOOKUP(P236, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -31949,7 +31949,7 @@
       <c r="M237" t="s">
         <v>50</v>
       </c>
-      <c r="O237" s="6">
+      <c r="O237" s="5">
         <f>IF(P237&lt;&gt;"", VLOOKUP(P237, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32018,7 +32018,7 @@
       <c r="N238" t="s">
         <v>119</v>
       </c>
-      <c r="O238" s="6">
+      <c r="O238" s="5">
         <f>IF(P238&lt;&gt;"", VLOOKUP(P238, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -32081,7 +32081,7 @@
       <c r="M239" t="s">
         <v>25</v>
       </c>
-      <c r="O239" s="6">
+      <c r="O239" s="5">
         <f>IF(P239&lt;&gt;"", VLOOKUP(P239, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -32150,7 +32150,7 @@
       <c r="M240" t="s">
         <v>50</v>
       </c>
-      <c r="O240" s="6">
+      <c r="O240" s="5">
         <f>IF(P240&lt;&gt;"", VLOOKUP(P240, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32216,7 +32216,7 @@
       <c r="M241" t="s">
         <v>50</v>
       </c>
-      <c r="O241" s="6">
+      <c r="O241" s="5">
         <f>IF(P241&lt;&gt;"", VLOOKUP(P241, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32285,7 +32285,7 @@
       <c r="N242" t="s">
         <v>28</v>
       </c>
-      <c r="O242" s="6">
+      <c r="O242" s="5">
         <f>IF(P242&lt;&gt;"", VLOOKUP(P242, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -32360,7 +32360,7 @@
       <c r="N243" t="s">
         <v>119</v>
       </c>
-      <c r="O243" s="6">
+      <c r="O243" s="5">
         <f>IF(P243&lt;&gt;"", VLOOKUP(P243, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -32429,7 +32429,7 @@
       <c r="M244" t="s">
         <v>50</v>
       </c>
-      <c r="O244" s="6">
+      <c r="O244" s="5">
         <f>IF(P244&lt;&gt;"", VLOOKUP(P244, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32498,7 +32498,7 @@
       <c r="N245" t="s">
         <v>68</v>
       </c>
-      <c r="O245" s="6">
+      <c r="O245" s="5">
         <f>IF(P245&lt;&gt;"", VLOOKUP(P245, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -32567,7 +32567,7 @@
       <c r="M246" t="s">
         <v>50</v>
       </c>
-      <c r="O246" s="6">
+      <c r="O246" s="5">
         <f>IF(P246&lt;&gt;"", VLOOKUP(P246, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32636,7 +32636,7 @@
       <c r="N247" t="s">
         <v>68</v>
       </c>
-      <c r="O247" s="6">
+      <c r="O247" s="5">
         <f>IF(P247&lt;&gt;"", VLOOKUP(P247, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -32699,7 +32699,7 @@
       <c r="M248" t="s">
         <v>50</v>
       </c>
-      <c r="O248" s="6">
+      <c r="O248" s="5">
         <f>IF(P248&lt;&gt;"", VLOOKUP(P248, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32765,7 +32765,7 @@
       <c r="M249" t="s">
         <v>50</v>
       </c>
-      <c r="O249" s="6">
+      <c r="O249" s="5">
         <f>IF(P249&lt;&gt;"", VLOOKUP(P249, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32831,7 +32831,7 @@
       <c r="M250" t="s">
         <v>50</v>
       </c>
-      <c r="O250" s="6">
+      <c r="O250" s="5">
         <f>IF(P250&lt;&gt;"", VLOOKUP(P250, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32897,7 +32897,7 @@
       <c r="M251" t="s">
         <v>50</v>
       </c>
-      <c r="O251" s="6">
+      <c r="O251" s="5">
         <f>IF(P251&lt;&gt;"", VLOOKUP(P251, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -32957,7 +32957,7 @@
       <c r="M252" t="s">
         <v>25</v>
       </c>
-      <c r="O252" s="6">
+      <c r="O252" s="5">
         <f>IF(P252&lt;&gt;"", VLOOKUP(P252, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -33020,7 +33020,7 @@
       <c r="M253" t="s">
         <v>50</v>
       </c>
-      <c r="O253" s="6">
+      <c r="O253" s="5">
         <f>IF(P253&lt;&gt;"", VLOOKUP(P253, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33080,7 +33080,7 @@
       <c r="M254" t="s">
         <v>50</v>
       </c>
-      <c r="O254" s="6">
+      <c r="O254" s="5">
         <f>IF(P254&lt;&gt;"", VLOOKUP(P254, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33146,7 +33146,7 @@
       <c r="M255" t="s">
         <v>50</v>
       </c>
-      <c r="O255" s="6">
+      <c r="O255" s="5">
         <f>IF(P255&lt;&gt;"", VLOOKUP(P255, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33212,7 +33212,7 @@
       <c r="M256" t="s">
         <v>50</v>
       </c>
-      <c r="O256" s="6">
+      <c r="O256" s="5">
         <f>IF(P256&lt;&gt;"", VLOOKUP(P256, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33278,7 +33278,7 @@
       <c r="M257" t="s">
         <v>50</v>
       </c>
-      <c r="O257" s="6">
+      <c r="O257" s="5">
         <f>IF(P257&lt;&gt;"", VLOOKUP(P257, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33347,7 +33347,7 @@
       <c r="N258" t="s">
         <v>68</v>
       </c>
-      <c r="O258" s="6">
+      <c r="O258" s="5">
         <f>IF(P258&lt;&gt;"", VLOOKUP(P258, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -33410,7 +33410,7 @@
       <c r="M259" t="s">
         <v>50</v>
       </c>
-      <c r="O259" s="6">
+      <c r="O259" s="5">
         <f>IF(P259&lt;&gt;"", VLOOKUP(P259, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33476,7 +33476,7 @@
       <c r="M260" t="s">
         <v>50</v>
       </c>
-      <c r="O260" s="6">
+      <c r="O260" s="5">
         <f>IF(P260&lt;&gt;"", VLOOKUP(P260, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33545,7 +33545,7 @@
       <c r="N261" t="s">
         <v>68</v>
       </c>
-      <c r="O261" s="6">
+      <c r="O261" s="5">
         <f>IF(P261&lt;&gt;"", VLOOKUP(P261, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -33617,7 +33617,7 @@
       <c r="M262" t="s">
         <v>50</v>
       </c>
-      <c r="O262" s="6">
+      <c r="O262" s="5">
         <f>IF(P262&lt;&gt;"", VLOOKUP(P262, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33677,7 +33677,7 @@
       <c r="M263" t="s">
         <v>50</v>
       </c>
-      <c r="O263" s="6">
+      <c r="O263" s="5">
         <f>IF(P263&lt;&gt;"", VLOOKUP(P263, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -33746,7 +33746,7 @@
       <c r="N264" t="s">
         <v>28</v>
       </c>
-      <c r="O264" s="6">
+      <c r="O264" s="5">
         <f>IF(P264&lt;&gt;"", VLOOKUP(P264, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -33818,7 +33818,7 @@
       <c r="N265" t="s">
         <v>68</v>
       </c>
-      <c r="O265" s="6">
+      <c r="O265" s="5">
         <f>IF(P265&lt;&gt;"", VLOOKUP(P265, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -33890,7 +33890,7 @@
       <c r="N266" t="s">
         <v>28</v>
       </c>
-      <c r="O266" s="6">
+      <c r="O266" s="5">
         <f>IF(P266&lt;&gt;"", VLOOKUP(P266, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -33953,7 +33953,7 @@
       <c r="M267" t="s">
         <v>50</v>
       </c>
-      <c r="O267" s="6">
+      <c r="O267" s="5">
         <f>IF(P267&lt;&gt;"", VLOOKUP(P267, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34013,7 +34013,7 @@
       <c r="M268" t="s">
         <v>50</v>
       </c>
-      <c r="O268" s="6">
+      <c r="O268" s="5">
         <f>IF(P268&lt;&gt;"", VLOOKUP(P268, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34079,7 +34079,7 @@
       <c r="M269" t="s">
         <v>50</v>
       </c>
-      <c r="O269" s="6">
+      <c r="O269" s="5">
         <f>IF(P269&lt;&gt;"", VLOOKUP(P269, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34139,7 +34139,7 @@
       <c r="M270" t="s">
         <v>50</v>
       </c>
-      <c r="O270" s="6">
+      <c r="O270" s="5">
         <f>IF(P270&lt;&gt;"", VLOOKUP(P270, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34205,7 +34205,7 @@
       <c r="M271" t="s">
         <v>50</v>
       </c>
-      <c r="O271" s="6">
+      <c r="O271" s="5">
         <f>IF(P271&lt;&gt;"", VLOOKUP(P271, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34274,7 +34274,7 @@
       <c r="N272" t="s">
         <v>51</v>
       </c>
-      <c r="O272" s="6">
+      <c r="O272" s="5">
         <f>IF(P272&lt;&gt;"", VLOOKUP(P272, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -34346,7 +34346,7 @@
       <c r="N273" t="s">
         <v>28</v>
       </c>
-      <c r="O273" s="6">
+      <c r="O273" s="5">
         <f>IF(P273&lt;&gt;"", VLOOKUP(P273, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -34409,7 +34409,7 @@
       <c r="M274" t="s">
         <v>50</v>
       </c>
-      <c r="O274" s="6">
+      <c r="O274" s="5">
         <f>IF(P274&lt;&gt;"", VLOOKUP(P274, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34475,7 +34475,7 @@
       <c r="M275" t="s">
         <v>50</v>
       </c>
-      <c r="O275" s="6">
+      <c r="O275" s="5">
         <f>IF(P275&lt;&gt;"", VLOOKUP(P275, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34535,7 +34535,7 @@
       <c r="M276" t="s">
         <v>50</v>
       </c>
-      <c r="O276" s="6">
+      <c r="O276" s="5">
         <f>IF(P276&lt;&gt;"", VLOOKUP(P276, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34601,7 +34601,7 @@
       <c r="M277" t="s">
         <v>50</v>
       </c>
-      <c r="O277" s="6">
+      <c r="O277" s="5">
         <f>IF(P277&lt;&gt;"", VLOOKUP(P277, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34670,7 +34670,7 @@
       <c r="N278" t="s">
         <v>51</v>
       </c>
-      <c r="O278" s="6">
+      <c r="O278" s="5">
         <f>IF(P278&lt;&gt;"", VLOOKUP(P278, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34739,7 +34739,7 @@
       <c r="M279" t="s">
         <v>50</v>
       </c>
-      <c r="O279" s="6">
+      <c r="O279" s="5">
         <f>IF(P279&lt;&gt;"", VLOOKUP(P279, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34805,7 +34805,7 @@
       <c r="M280" t="s">
         <v>50</v>
       </c>
-      <c r="O280" s="6">
+      <c r="O280" s="5">
         <f>IF(P280&lt;&gt;"", VLOOKUP(P280, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34871,7 +34871,7 @@
       <c r="M281" t="s">
         <v>50</v>
       </c>
-      <c r="O281" s="6">
+      <c r="O281" s="5">
         <f>IF(P281&lt;&gt;"", VLOOKUP(P281, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -34931,7 +34931,7 @@
       <c r="M282" t="s">
         <v>25</v>
       </c>
-      <c r="O282" s="6">
+      <c r="O282" s="5">
         <f>IF(P282&lt;&gt;"", VLOOKUP(P282, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35000,7 +35000,7 @@
       <c r="M283" t="s">
         <v>50</v>
       </c>
-      <c r="O283" s="6">
+      <c r="O283" s="5">
         <f>IF(P283&lt;&gt;"", VLOOKUP(P283, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35069,7 +35069,7 @@
       <c r="N284" t="s">
         <v>28</v>
       </c>
-      <c r="O284" s="6">
+      <c r="O284" s="5">
         <f>IF(P284&lt;&gt;"", VLOOKUP(P284, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35141,7 +35141,7 @@
       <c r="N285" t="s">
         <v>68</v>
       </c>
-      <c r="O285" s="6">
+      <c r="O285" s="5">
         <f>IF(P285&lt;&gt;"", VLOOKUP(P285, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35204,7 +35204,7 @@
       <c r="M286" t="s">
         <v>25</v>
       </c>
-      <c r="O286" s="6">
+      <c r="O286" s="5">
         <f>IF(P286&lt;&gt;"", VLOOKUP(P286, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35276,7 +35276,7 @@
       <c r="N287" t="s">
         <v>68</v>
       </c>
-      <c r="O287" s="6">
+      <c r="O287" s="5">
         <f>IF(P287&lt;&gt;"", VLOOKUP(P287, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35348,7 +35348,7 @@
       <c r="N288" t="s">
         <v>28</v>
       </c>
-      <c r="O288" s="6">
+      <c r="O288" s="5">
         <f>IF(P288&lt;&gt;"", VLOOKUP(P288, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -35417,7 +35417,7 @@
       <c r="M289" t="s">
         <v>50</v>
       </c>
-      <c r="O289" s="6">
+      <c r="O289" s="5">
         <f>IF(P289&lt;&gt;"", VLOOKUP(P289, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35486,7 +35486,7 @@
       <c r="N290" t="s">
         <v>28</v>
       </c>
-      <c r="O290" s="6">
+      <c r="O290" s="5">
         <f>IF(P290&lt;&gt;"", VLOOKUP(P290, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -35549,7 +35549,7 @@
       <c r="M291" t="s">
         <v>50</v>
       </c>
-      <c r="O291" s="6">
+      <c r="O291" s="5">
         <f>IF(P291&lt;&gt;"", VLOOKUP(P291, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35615,7 +35615,7 @@
       <c r="M292" t="s">
         <v>50</v>
       </c>
-      <c r="O292" s="6">
+      <c r="O292" s="5">
         <f>IF(P292&lt;&gt;"", VLOOKUP(P292, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35684,7 +35684,7 @@
       <c r="N293" t="s">
         <v>28</v>
       </c>
-      <c r="O293" s="6">
+      <c r="O293" s="5">
         <f>IF(P293&lt;&gt;"", VLOOKUP(P293, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -35753,7 +35753,7 @@
       <c r="M294" t="s">
         <v>50</v>
       </c>
-      <c r="O294" s="6">
+      <c r="O294" s="5">
         <f>IF(P294&lt;&gt;"", VLOOKUP(P294, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35813,7 +35813,7 @@
       <c r="M295" t="s">
         <v>50</v>
       </c>
-      <c r="O295" s="6">
+      <c r="O295" s="5">
         <f>IF(P295&lt;&gt;"", VLOOKUP(P295, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35879,7 +35879,7 @@
       <c r="M296" t="s">
         <v>50</v>
       </c>
-      <c r="O296" s="6">
+      <c r="O296" s="5">
         <f>IF(P296&lt;&gt;"", VLOOKUP(P296, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -35939,7 +35939,7 @@
       <c r="M297" t="s">
         <v>50</v>
       </c>
-      <c r="O297" s="6">
+      <c r="O297" s="5">
         <f>IF(P297&lt;&gt;"", VLOOKUP(P297, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36005,7 +36005,7 @@
       <c r="M298" t="s">
         <v>50</v>
       </c>
-      <c r="O298" s="6">
+      <c r="O298" s="5">
         <f>IF(P298&lt;&gt;"", VLOOKUP(P298, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36074,7 +36074,7 @@
       <c r="N299" t="s">
         <v>28</v>
       </c>
-      <c r="O299" s="6">
+      <c r="O299" s="5">
         <f>IF(P299&lt;&gt;"", VLOOKUP(P299, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -36143,7 +36143,7 @@
       <c r="M300" t="s">
         <v>50</v>
       </c>
-      <c r="O300" s="6">
+      <c r="O300" s="5">
         <f>IF(P300&lt;&gt;"", VLOOKUP(P300, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36212,7 +36212,7 @@
       <c r="N301" t="s">
         <v>28</v>
       </c>
-      <c r="O301" s="6">
+      <c r="O301" s="5">
         <f>IF(P301&lt;&gt;"", VLOOKUP(P301, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -36275,7 +36275,7 @@
       <c r="M302" t="s">
         <v>50</v>
       </c>
-      <c r="O302" s="6">
+      <c r="O302" s="5">
         <f>IF(P302&lt;&gt;"", VLOOKUP(P302, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36344,7 +36344,7 @@
       <c r="N303" t="s">
         <v>28</v>
       </c>
-      <c r="O303" s="6">
+      <c r="O303" s="5">
         <f>IF(P303&lt;&gt;"", VLOOKUP(P303, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -36413,7 +36413,7 @@
       <c r="M304" t="s">
         <v>50</v>
       </c>
-      <c r="O304" s="6">
+      <c r="O304" s="5">
         <f>IF(P304&lt;&gt;"", VLOOKUP(P304, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36482,7 +36482,7 @@
       <c r="M305" t="s">
         <v>50</v>
       </c>
-      <c r="O305" s="6">
+      <c r="O305" s="5">
         <f>IF(P305&lt;&gt;"", VLOOKUP(P305, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36551,7 +36551,7 @@
       <c r="N306" t="s">
         <v>68</v>
       </c>
-      <c r="O306" s="6">
+      <c r="O306" s="5">
         <f>IF(P306&lt;&gt;"", VLOOKUP(P306, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -36623,7 +36623,7 @@
       <c r="N307" t="s">
         <v>68</v>
       </c>
-      <c r="O307" s="6">
+      <c r="O307" s="5">
         <f>IF(P307&lt;&gt;"", VLOOKUP(P307, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -36695,7 +36695,7 @@
       <c r="N308" t="s">
         <v>28</v>
       </c>
-      <c r="O308" s="6">
+      <c r="O308" s="5">
         <f>IF(P308&lt;&gt;"", VLOOKUP(P308, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -36764,7 +36764,7 @@
       <c r="M309" t="s">
         <v>50</v>
       </c>
-      <c r="O309" s="6">
+      <c r="O309" s="5">
         <f>IF(P309&lt;&gt;"", VLOOKUP(P309, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36830,7 +36830,7 @@
       <c r="M310" t="s">
         <v>50</v>
       </c>
-      <c r="O310" s="6">
+      <c r="O310" s="5">
         <f>IF(P310&lt;&gt;"", VLOOKUP(P310, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36896,7 +36896,7 @@
       <c r="M311" t="s">
         <v>50</v>
       </c>
-      <c r="O311" s="6">
+      <c r="O311" s="5">
         <f>IF(P311&lt;&gt;"", VLOOKUP(P311, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -36956,7 +36956,7 @@
       <c r="M312" t="s">
         <v>50</v>
       </c>
-      <c r="O312" s="6">
+      <c r="O312" s="5">
         <f>IF(P312&lt;&gt;"", VLOOKUP(P312, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37025,7 +37025,7 @@
       <c r="N313" t="s">
         <v>68</v>
       </c>
-      <c r="O313" s="6">
+      <c r="O313" s="5">
         <f>IF(P313&lt;&gt;"", VLOOKUP(P313, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -37097,7 +37097,7 @@
       <c r="N314" t="s">
         <v>28</v>
       </c>
-      <c r="O314" s="6">
+      <c r="O314" s="5">
         <f>IF(P314&lt;&gt;"", VLOOKUP(P314, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -37166,7 +37166,7 @@
       <c r="M315" t="s">
         <v>50</v>
       </c>
-      <c r="O315" s="6">
+      <c r="O315" s="5">
         <f>IF(P315&lt;&gt;"", VLOOKUP(P315, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37232,7 +37232,7 @@
       <c r="M316" t="s">
         <v>50</v>
       </c>
-      <c r="O316" s="6">
+      <c r="O316" s="5">
         <f>IF(P316&lt;&gt;"", VLOOKUP(P316, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37301,7 +37301,7 @@
       <c r="N317" t="s">
         <v>119</v>
       </c>
-      <c r="O317" s="6">
+      <c r="O317" s="5">
         <f>IF(P317&lt;&gt;"", VLOOKUP(P317, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -37370,7 +37370,7 @@
       <c r="M318" t="s">
         <v>50</v>
       </c>
-      <c r="O318" s="6">
+      <c r="O318" s="5">
         <f>IF(P318&lt;&gt;"", VLOOKUP(P318, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37436,7 +37436,7 @@
       <c r="M319" t="s">
         <v>50</v>
       </c>
-      <c r="O319" s="6">
+      <c r="O319" s="5">
         <f>IF(P319&lt;&gt;"", VLOOKUP(P319, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37496,7 +37496,7 @@
       <c r="M320" t="s">
         <v>50</v>
       </c>
-      <c r="O320" s="6">
+      <c r="O320" s="5">
         <f>IF(P320&lt;&gt;"", VLOOKUP(P320, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37565,7 +37565,7 @@
       <c r="N321" t="s">
         <v>28</v>
       </c>
-      <c r="O321" s="6">
+      <c r="O321" s="5">
         <f>IF(P321&lt;&gt;"", VLOOKUP(P321, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -37634,7 +37634,7 @@
       <c r="M322" t="s">
         <v>50</v>
       </c>
-      <c r="O322" s="6">
+      <c r="O322" s="5">
         <f>IF(P322&lt;&gt;"", VLOOKUP(P322, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37703,7 +37703,7 @@
       <c r="N323" t="s">
         <v>28</v>
       </c>
-      <c r="O323" s="6">
+      <c r="O323" s="5">
         <f>IF(P323&lt;&gt;"", VLOOKUP(P323, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -37772,7 +37772,7 @@
       <c r="M324" t="s">
         <v>50</v>
       </c>
-      <c r="O324" s="6">
+      <c r="O324" s="5">
         <f>IF(P324&lt;&gt;"", VLOOKUP(P324, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37838,7 +37838,7 @@
       <c r="M325" t="s">
         <v>50</v>
       </c>
-      <c r="O325" s="6">
+      <c r="O325" s="5">
         <f>IF(P325&lt;&gt;"", VLOOKUP(P325, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -37907,7 +37907,7 @@
       <c r="N326" t="s">
         <v>68</v>
       </c>
-      <c r="O326" s="6">
+      <c r="O326" s="5">
         <f>IF(P326&lt;&gt;"", VLOOKUP(P326, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -37979,7 +37979,7 @@
       <c r="N327" t="s">
         <v>68</v>
       </c>
-      <c r="O327" s="6">
+      <c r="O327" s="5">
         <f>IF(P327&lt;&gt;"", VLOOKUP(P327, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>4</v>
       </c>
@@ -38051,7 +38051,7 @@
       <c r="N328" t="s">
         <v>119</v>
       </c>
-      <c r="O328" s="6">
+      <c r="O328" s="5">
         <f>IF(P328&lt;&gt;"", VLOOKUP(P328, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -38120,7 +38120,7 @@
       <c r="M329" t="s">
         <v>50</v>
       </c>
-      <c r="O329" s="6">
+      <c r="O329" s="5">
         <f>IF(P329&lt;&gt;"", VLOOKUP(P329, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -38189,7 +38189,7 @@
       <c r="N330" t="s">
         <v>119</v>
       </c>
-      <c r="O330" s="6">
+      <c r="O330" s="5">
         <f>IF(P330&lt;&gt;"", VLOOKUP(P330, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -38258,7 +38258,7 @@
       <c r="M331" t="s">
         <v>50</v>
       </c>
-      <c r="O331" s="6">
+      <c r="O331" s="5">
         <f>IF(P331&lt;&gt;"", VLOOKUP(P331, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -38318,7 +38318,7 @@
       <c r="M332" t="s">
         <v>25</v>
       </c>
-      <c r="O332" s="6">
+      <c r="O332" s="5">
         <f>IF(P332&lt;&gt;"", VLOOKUP(P332, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -38390,7 +38390,7 @@
       <c r="N333" t="s">
         <v>28</v>
       </c>
-      <c r="O333" s="6">
+      <c r="O333" s="5">
         <f>IF(P333&lt;&gt;"", VLOOKUP(P333, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -38462,7 +38462,7 @@
       <c r="N334" t="s">
         <v>68</v>
       </c>
-      <c r="O334" s="6">
+      <c r="O334" s="5">
         <f>IF(P334&lt;&gt;"", VLOOKUP(P334, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -38534,7 +38534,7 @@
       <c r="N335" t="s">
         <v>68</v>
       </c>
-      <c r="O335" s="6">
+      <c r="O335" s="5">
         <f>IF(P335&lt;&gt;"", VLOOKUP(P335, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -38606,7 +38606,7 @@
       <c r="N336" t="s">
         <v>119</v>
       </c>
-      <c r="O336" s="6">
+      <c r="O336" s="5">
         <f>IF(P336&lt;&gt;"", VLOOKUP(P336, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -38669,7 +38669,7 @@
       <c r="M337" t="s">
         <v>25</v>
       </c>
-      <c r="O337" s="6">
+      <c r="O337" s="5">
         <f>IF(P337&lt;&gt;"", VLOOKUP(P337, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -38738,7 +38738,7 @@
       <c r="M338" t="s">
         <v>50</v>
       </c>
-      <c r="O338" s="6">
+      <c r="O338" s="5">
         <f>IF(P338&lt;&gt;"", VLOOKUP(P338, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -38798,7 +38798,7 @@
       <c r="M339" t="s">
         <v>25</v>
       </c>
-      <c r="O339" s="6">
+      <c r="O339" s="5">
         <f>IF(P339&lt;&gt;"", VLOOKUP(P339, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -38861,7 +38861,7 @@
       <c r="M340" t="s">
         <v>50</v>
       </c>
-      <c r="O340" s="6">
+      <c r="O340" s="5">
         <f>IF(P340&lt;&gt;"", VLOOKUP(P340, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -38927,7 +38927,7 @@
       <c r="M341" t="s">
         <v>50</v>
       </c>
-      <c r="O341" s="6">
+      <c r="O341" s="5">
         <f>IF(P341&lt;&gt;"", VLOOKUP(P341, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -38993,7 +38993,7 @@
       <c r="M342" t="s">
         <v>50</v>
       </c>
-      <c r="O342" s="6">
+      <c r="O342" s="5">
         <f>IF(P342&lt;&gt;"", VLOOKUP(P342, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39062,7 +39062,7 @@
       <c r="N343" t="s">
         <v>28</v>
       </c>
-      <c r="O343" s="6">
+      <c r="O343" s="5">
         <f>IF(P343&lt;&gt;"", VLOOKUP(P343, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -39131,7 +39131,7 @@
       <c r="M344" t="s">
         <v>50</v>
       </c>
-      <c r="O344" s="6">
+      <c r="O344" s="5">
         <f>IF(P344&lt;&gt;"", VLOOKUP(P344, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39200,7 +39200,7 @@
       <c r="N345" t="s">
         <v>68</v>
       </c>
-      <c r="O345" s="6">
+      <c r="O345" s="5">
         <f>IF(P345&lt;&gt;"", VLOOKUP(P345, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -39269,7 +39269,7 @@
       <c r="M346" t="s">
         <v>50</v>
       </c>
-      <c r="O346" s="6">
+      <c r="O346" s="5">
         <f>IF(P346&lt;&gt;"", VLOOKUP(P346, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39338,7 +39338,7 @@
       <c r="N347" t="s">
         <v>68</v>
       </c>
-      <c r="O347" s="6">
+      <c r="O347" s="5">
         <f>IF(P347&lt;&gt;"", VLOOKUP(P347, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -39410,7 +39410,7 @@
       <c r="N348" t="s">
         <v>68</v>
       </c>
-      <c r="O348" s="6">
+      <c r="O348" s="5">
         <f>IF(P348&lt;&gt;"", VLOOKUP(P348, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -39479,7 +39479,7 @@
       <c r="M349" t="s">
         <v>50</v>
       </c>
-      <c r="O349" s="6">
+      <c r="O349" s="5">
         <f>IF(P349&lt;&gt;"", VLOOKUP(P349, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39548,7 +39548,7 @@
       <c r="N350" t="s">
         <v>68</v>
       </c>
-      <c r="O350" s="6">
+      <c r="O350" s="5">
         <f>IF(P350&lt;&gt;"", VLOOKUP(P350, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -39620,7 +39620,7 @@
       <c r="N351" t="s">
         <v>28</v>
       </c>
-      <c r="O351" s="6">
+      <c r="O351" s="5">
         <f>IF(P351&lt;&gt;"", VLOOKUP(P351, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -39689,7 +39689,7 @@
       <c r="M352" t="s">
         <v>50</v>
       </c>
-      <c r="O352" s="6">
+      <c r="O352" s="5">
         <f>IF(P352&lt;&gt;"", VLOOKUP(P352, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39755,7 +39755,7 @@
       <c r="M353" t="s">
         <v>50</v>
       </c>
-      <c r="O353" s="6">
+      <c r="O353" s="5">
         <f>IF(P353&lt;&gt;"", VLOOKUP(P353, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39821,7 +39821,7 @@
       <c r="M354" t="s">
         <v>50</v>
       </c>
-      <c r="O354" s="6">
+      <c r="O354" s="5">
         <f>IF(P354&lt;&gt;"", VLOOKUP(P354, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39881,7 +39881,7 @@
       <c r="M355" t="s">
         <v>50</v>
       </c>
-      <c r="O355" s="6">
+      <c r="O355" s="5">
         <f>IF(P355&lt;&gt;"", VLOOKUP(P355, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -39950,7 +39950,7 @@
       <c r="N356" t="s">
         <v>119</v>
       </c>
-      <c r="O356" s="6">
+      <c r="O356" s="5">
         <f>IF(P356&lt;&gt;"", VLOOKUP(P356, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -40019,7 +40019,7 @@
       <c r="M357" t="s">
         <v>50</v>
       </c>
-      <c r="O357" s="6">
+      <c r="O357" s="5">
         <f>IF(P357&lt;&gt;"", VLOOKUP(P357, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40085,7 +40085,7 @@
       <c r="M358" t="s">
         <v>50</v>
       </c>
-      <c r="O358" s="6">
+      <c r="O358" s="5">
         <f>IF(P358&lt;&gt;"", VLOOKUP(P358, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40151,7 +40151,7 @@
       <c r="M359" t="s">
         <v>50</v>
       </c>
-      <c r="O359" s="6">
+      <c r="O359" s="5">
         <f>IF(P359&lt;&gt;"", VLOOKUP(P359, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40217,7 +40217,7 @@
       <c r="M360" t="s">
         <v>50</v>
       </c>
-      <c r="O360" s="6">
+      <c r="O360" s="5">
         <f>IF(P360&lt;&gt;"", VLOOKUP(P360, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40283,7 +40283,7 @@
       <c r="M361" t="s">
         <v>50</v>
       </c>
-      <c r="O361" s="6">
+      <c r="O361" s="5">
         <f>IF(P361&lt;&gt;"", VLOOKUP(P361, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40343,7 +40343,7 @@
       <c r="M362" t="s">
         <v>50</v>
       </c>
-      <c r="O362" s="6">
+      <c r="O362" s="5">
         <f>IF(P362&lt;&gt;"", VLOOKUP(P362, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40409,7 +40409,7 @@
       <c r="M363" t="s">
         <v>50</v>
       </c>
-      <c r="O363" s="6">
+      <c r="O363" s="5">
         <f>IF(P363&lt;&gt;"", VLOOKUP(P363, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40475,7 +40475,7 @@
       <c r="M364" t="s">
         <v>50</v>
       </c>
-      <c r="O364" s="6">
+      <c r="O364" s="5">
         <f>IF(P364&lt;&gt;"", VLOOKUP(P364, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40535,7 +40535,7 @@
       <c r="M365" t="s">
         <v>25</v>
       </c>
-      <c r="O365" s="6">
+      <c r="O365" s="5">
         <f>IF(P365&lt;&gt;"", VLOOKUP(P365, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -40604,7 +40604,7 @@
       <c r="M366" t="s">
         <v>50</v>
       </c>
-      <c r="O366" s="6">
+      <c r="O366" s="5">
         <f>IF(P366&lt;&gt;"", VLOOKUP(P366, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40664,7 +40664,7 @@
       <c r="M367" t="s">
         <v>50</v>
       </c>
-      <c r="O367" s="6">
+      <c r="O367" s="5">
         <f>IF(P367&lt;&gt;"", VLOOKUP(P367, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40730,7 +40730,7 @@
       <c r="M368" t="s">
         <v>50</v>
       </c>
-      <c r="O368" s="6">
+      <c r="O368" s="5">
         <f>IF(P368&lt;&gt;"", VLOOKUP(P368, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40799,7 +40799,7 @@
       <c r="N369" t="s">
         <v>119</v>
       </c>
-      <c r="O369" s="6">
+      <c r="O369" s="5">
         <f>IF(P369&lt;&gt;"", VLOOKUP(P369, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -40868,7 +40868,7 @@
       <c r="M370" t="s">
         <v>50</v>
       </c>
-      <c r="O370" s="6">
+      <c r="O370" s="5">
         <f>IF(P370&lt;&gt;"", VLOOKUP(P370, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -40937,7 +40937,7 @@
       <c r="N371" t="s">
         <v>68</v>
       </c>
-      <c r="O371" s="6">
+      <c r="O371" s="5">
         <f>IF(P371&lt;&gt;"", VLOOKUP(P371, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -41009,7 +41009,7 @@
       <c r="N372" t="s">
         <v>68</v>
       </c>
-      <c r="O372" s="6">
+      <c r="O372" s="5">
         <f>IF(P372&lt;&gt;"", VLOOKUP(P372, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -41078,7 +41078,7 @@
       <c r="M373" t="s">
         <v>50</v>
       </c>
-      <c r="O373" s="6">
+      <c r="O373" s="5">
         <f>IF(P373&lt;&gt;"", VLOOKUP(P373, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41144,7 +41144,7 @@
       <c r="M374" t="s">
         <v>50</v>
       </c>
-      <c r="O374" s="6">
+      <c r="O374" s="5">
         <f>IF(P374&lt;&gt;"", VLOOKUP(P374, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41210,7 +41210,7 @@
       <c r="M375" t="s">
         <v>50</v>
       </c>
-      <c r="O375" s="6">
+      <c r="O375" s="5">
         <f>IF(P375&lt;&gt;"", VLOOKUP(P375, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41279,7 +41279,7 @@
       <c r="N376" t="s">
         <v>68</v>
       </c>
-      <c r="O376" s="6">
+      <c r="O376" s="5">
         <f>IF(P376&lt;&gt;"", VLOOKUP(P376, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41348,7 +41348,7 @@
       <c r="M377" t="s">
         <v>50</v>
       </c>
-      <c r="O377" s="6">
+      <c r="O377" s="5">
         <f>IF(P377&lt;&gt;"", VLOOKUP(P377, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41408,7 +41408,7 @@
       <c r="M378" t="s">
         <v>25</v>
       </c>
-      <c r="O378" s="6">
+      <c r="O378" s="5">
         <f>IF(P378&lt;&gt;"", VLOOKUP(P378, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -41477,7 +41477,7 @@
       <c r="M379" t="s">
         <v>50</v>
       </c>
-      <c r="O379" s="6">
+      <c r="O379" s="5">
         <f>IF(P379&lt;&gt;"", VLOOKUP(P379, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41537,7 +41537,7 @@
       <c r="M380" t="s">
         <v>50</v>
       </c>
-      <c r="O380" s="6">
+      <c r="O380" s="5">
         <f>IF(P380&lt;&gt;"", VLOOKUP(P380, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41597,7 +41597,7 @@
       <c r="M381" t="s">
         <v>25</v>
       </c>
-      <c r="O381" s="6">
+      <c r="O381" s="5">
         <f>IF(P381&lt;&gt;"", VLOOKUP(P381, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -41669,7 +41669,7 @@
       <c r="N382" t="s">
         <v>28</v>
       </c>
-      <c r="O382" s="6">
+      <c r="O382" s="5">
         <f>IF(P382&lt;&gt;"", VLOOKUP(P382, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -41741,7 +41741,7 @@
       <c r="N383" t="s">
         <v>28</v>
       </c>
-      <c r="O383" s="6">
+      <c r="O383" s="5">
         <f>IF(P383&lt;&gt;"", VLOOKUP(P383, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -41804,7 +41804,7 @@
       <c r="M384" t="s">
         <v>50</v>
       </c>
-      <c r="O384" s="6">
+      <c r="O384" s="5">
         <f>IF(P384&lt;&gt;"", VLOOKUP(P384, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -41873,7 +41873,7 @@
       <c r="N385" t="s">
         <v>28</v>
       </c>
-      <c r="O385" s="6">
+      <c r="O385" s="5">
         <f>IF(P385&lt;&gt;"", VLOOKUP(P385, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>4</v>
       </c>
@@ -41945,7 +41945,7 @@
       <c r="N386" t="s">
         <v>28</v>
       </c>
-      <c r="O386" s="6">
+      <c r="O386" s="5">
         <f>IF(P386&lt;&gt;"", VLOOKUP(P386, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -42014,7 +42014,7 @@
       <c r="M387" t="s">
         <v>50</v>
       </c>
-      <c r="O387" s="6">
+      <c r="O387" s="5">
         <f>IF(P387&lt;&gt;"", VLOOKUP(P387, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42080,7 +42080,7 @@
       <c r="M388" t="s">
         <v>50</v>
       </c>
-      <c r="O388" s="6">
+      <c r="O388" s="5">
         <f>IF(P388&lt;&gt;"", VLOOKUP(P388, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42146,7 +42146,7 @@
       <c r="M389" t="s">
         <v>50</v>
       </c>
-      <c r="O389" s="6">
+      <c r="O389" s="5">
         <f>IF(P389&lt;&gt;"", VLOOKUP(P389, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42218,7 +42218,7 @@
       <c r="N390" t="s">
         <v>119</v>
       </c>
-      <c r="O390" s="6">
+      <c r="O390" s="5">
         <f>IF(P390&lt;&gt;"", VLOOKUP(P390, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -42284,7 +42284,7 @@
       <c r="M391" t="s">
         <v>50</v>
       </c>
-      <c r="O391" s="6">
+      <c r="O391" s="5">
         <f>IF(P391&lt;&gt;"", VLOOKUP(P391, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42353,7 +42353,7 @@
       <c r="N392" t="s">
         <v>119</v>
       </c>
-      <c r="O392" s="6">
+      <c r="O392" s="5">
         <f>IF(P392&lt;&gt;"", VLOOKUP(P392, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -42416,7 +42416,7 @@
       <c r="M393" t="s">
         <v>50</v>
       </c>
-      <c r="O393" s="6">
+      <c r="O393" s="5">
         <f>IF(P393&lt;&gt;"", VLOOKUP(P393, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42485,7 +42485,7 @@
       <c r="N394" t="s">
         <v>28</v>
       </c>
-      <c r="O394" s="6">
+      <c r="O394" s="5">
         <f>IF(P394&lt;&gt;"", VLOOKUP(P394, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -42557,7 +42557,7 @@
       <c r="N395" t="s">
         <v>28</v>
       </c>
-      <c r="O395" s="6">
+      <c r="O395" s="5">
         <f>IF(P395&lt;&gt;"", VLOOKUP(P395, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -42626,7 +42626,7 @@
       <c r="M396" t="s">
         <v>50</v>
       </c>
-      <c r="O396" s="6">
+      <c r="O396" s="5">
         <f>IF(P396&lt;&gt;"", VLOOKUP(P396, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42692,7 +42692,7 @@
       <c r="M397" t="s">
         <v>50</v>
       </c>
-      <c r="O397" s="6">
+      <c r="O397" s="5">
         <f>IF(P397&lt;&gt;"", VLOOKUP(P397, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42758,7 +42758,7 @@
       <c r="M398" t="s">
         <v>50</v>
       </c>
-      <c r="O398" s="6">
+      <c r="O398" s="5">
         <f>IF(P398&lt;&gt;"", VLOOKUP(P398, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42827,7 +42827,7 @@
       <c r="N399" t="s">
         <v>28</v>
       </c>
-      <c r="O399" s="6">
+      <c r="O399" s="5">
         <f>IF(P399&lt;&gt;"", VLOOKUP(P399, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -42896,7 +42896,7 @@
       <c r="M400" t="s">
         <v>50</v>
       </c>
-      <c r="O400" s="6">
+      <c r="O400" s="5">
         <f>IF(P400&lt;&gt;"", VLOOKUP(P400, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -42965,7 +42965,7 @@
       <c r="N401" t="s">
         <v>68</v>
       </c>
-      <c r="O401" s="6">
+      <c r="O401" s="5">
         <f>IF(P401&lt;&gt;"", VLOOKUP(P401, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -43034,7 +43034,7 @@
       <c r="M402" t="s">
         <v>50</v>
       </c>
-      <c r="O402" s="6">
+      <c r="O402" s="5">
         <f>IF(P402&lt;&gt;"", VLOOKUP(P402, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43100,7 +43100,7 @@
       <c r="M403" t="s">
         <v>50</v>
       </c>
-      <c r="O403" s="6">
+      <c r="O403" s="5">
         <f>IF(P403&lt;&gt;"", VLOOKUP(P403, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43160,7 +43160,7 @@
       <c r="M404" t="s">
         <v>50</v>
       </c>
-      <c r="O404" s="6">
+      <c r="O404" s="5">
         <f>IF(P404&lt;&gt;"", VLOOKUP(P404, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43229,7 +43229,7 @@
       <c r="N405" t="s">
         <v>28</v>
       </c>
-      <c r="O405" s="6">
+      <c r="O405" s="5">
         <f>IF(P405&lt;&gt;"", VLOOKUP(P405, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -43292,7 +43292,7 @@
       <c r="M406" t="s">
         <v>50</v>
       </c>
-      <c r="O406" s="6">
+      <c r="O406" s="5">
         <f>IF(P406&lt;&gt;"", VLOOKUP(P406, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43352,7 +43352,7 @@
       <c r="M407" t="s">
         <v>50</v>
       </c>
-      <c r="O407" s="6">
+      <c r="O407" s="5">
         <f>IF(P407&lt;&gt;"", VLOOKUP(P407, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43412,7 +43412,7 @@
       <c r="M408" t="s">
         <v>50</v>
       </c>
-      <c r="O408" s="6">
+      <c r="O408" s="5">
         <f>IF(P408&lt;&gt;"", VLOOKUP(P408, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43472,7 +43472,7 @@
       <c r="M409" t="s">
         <v>25</v>
       </c>
-      <c r="O409" s="6">
+      <c r="O409" s="5">
         <f>IF(P409&lt;&gt;"", VLOOKUP(P409, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -43541,7 +43541,7 @@
       <c r="M410" t="s">
         <v>50</v>
       </c>
-      <c r="O410" s="6">
+      <c r="O410" s="5">
         <f>IF(P410&lt;&gt;"", VLOOKUP(P410, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43601,7 +43601,7 @@
       <c r="M411" t="s">
         <v>50</v>
       </c>
-      <c r="O411" s="6">
+      <c r="O411" s="5">
         <f>IF(P411&lt;&gt;"", VLOOKUP(P411, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43667,7 +43667,7 @@
       <c r="M412" t="s">
         <v>50</v>
       </c>
-      <c r="O412" s="6">
+      <c r="O412" s="5">
         <f>IF(P412&lt;&gt;"", VLOOKUP(P412, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43727,7 +43727,7 @@
       <c r="M413" t="s">
         <v>50</v>
       </c>
-      <c r="O413" s="6">
+      <c r="O413" s="5">
         <f>IF(P413&lt;&gt;"", VLOOKUP(P413, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43787,7 +43787,7 @@
       <c r="M414" t="s">
         <v>25</v>
       </c>
-      <c r="O414" s="6">
+      <c r="O414" s="5">
         <f>IF(P414&lt;&gt;"", VLOOKUP(P414, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -43856,7 +43856,7 @@
       <c r="M415" t="s">
         <v>50</v>
       </c>
-      <c r="O415" s="6">
+      <c r="O415" s="5">
         <f>IF(P415&lt;&gt;"", VLOOKUP(P415, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43922,7 +43922,7 @@
       <c r="M416" t="s">
         <v>50</v>
       </c>
-      <c r="O416" s="6">
+      <c r="O416" s="5">
         <f>IF(P416&lt;&gt;"", VLOOKUP(P416, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -43988,7 +43988,7 @@
       <c r="M417" t="s">
         <v>50</v>
       </c>
-      <c r="O417" s="6">
+      <c r="O417" s="5">
         <f>IF(P417&lt;&gt;"", VLOOKUP(P417, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44048,7 +44048,7 @@
       <c r="M418" t="s">
         <v>50</v>
       </c>
-      <c r="O418" s="6">
+      <c r="O418" s="5">
         <f>IF(P418&lt;&gt;"", VLOOKUP(P418, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44114,7 +44114,7 @@
       <c r="M419" t="s">
         <v>50</v>
       </c>
-      <c r="O419" s="6">
+      <c r="O419" s="5">
         <f>IF(P419&lt;&gt;"", VLOOKUP(P419, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44183,7 +44183,7 @@
       <c r="N420" t="s">
         <v>119</v>
       </c>
-      <c r="O420" s="6">
+      <c r="O420" s="5">
         <f>IF(P420&lt;&gt;"", VLOOKUP(P420, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>4</v>
       </c>
@@ -44246,7 +44246,7 @@
       <c r="M421" t="s">
         <v>25</v>
       </c>
-      <c r="O421" s="6">
+      <c r="O421" s="5">
         <f>IF(P421&lt;&gt;"", VLOOKUP(P421, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -44315,7 +44315,7 @@
       <c r="M422" t="s">
         <v>50</v>
       </c>
-      <c r="O422" s="6">
+      <c r="O422" s="5">
         <f>IF(P422&lt;&gt;"", VLOOKUP(P422, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44384,7 +44384,7 @@
       <c r="N423" t="s">
         <v>28</v>
       </c>
-      <c r="O423" s="6">
+      <c r="O423" s="5">
         <f>IF(P423&lt;&gt;"", VLOOKUP(P423, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -44447,7 +44447,7 @@
       <c r="M424" t="s">
         <v>25</v>
       </c>
-      <c r="O424" s="6">
+      <c r="O424" s="5">
         <f>IF(P424&lt;&gt;"", VLOOKUP(P424, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -44516,7 +44516,7 @@
       <c r="M425" t="s">
         <v>50</v>
       </c>
-      <c r="O425" s="6">
+      <c r="O425" s="5">
         <f>IF(P425&lt;&gt;"", VLOOKUP(P425, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44576,7 +44576,7 @@
       <c r="M426" t="s">
         <v>25</v>
       </c>
-      <c r="O426" s="6">
+      <c r="O426" s="5">
         <f>IF(P426&lt;&gt;"", VLOOKUP(P426, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -44651,7 +44651,7 @@
       <c r="N427" t="s">
         <v>28</v>
       </c>
-      <c r="O427" s="6">
+      <c r="O427" s="5">
         <f>IF(P427&lt;&gt;"", VLOOKUP(P427, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -44714,7 +44714,7 @@
       <c r="M428" t="s">
         <v>25</v>
       </c>
-      <c r="O428" s="6">
+      <c r="O428" s="5">
         <f>IF(P428&lt;&gt;"", VLOOKUP(P428, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -44783,7 +44783,7 @@
       <c r="M429" t="s">
         <v>50</v>
       </c>
-      <c r="O429" s="6">
+      <c r="O429" s="5">
         <f>IF(P429&lt;&gt;"", VLOOKUP(P429, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44843,7 +44843,7 @@
       <c r="M430" t="s">
         <v>50</v>
       </c>
-      <c r="O430" s="6">
+      <c r="O430" s="5">
         <f>IF(P430&lt;&gt;"", VLOOKUP(P430, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -44912,7 +44912,7 @@
       <c r="N431" t="s">
         <v>119</v>
       </c>
-      <c r="O431" s="6">
+      <c r="O431" s="5">
         <f>IF(P431&lt;&gt;"", VLOOKUP(P431, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -44975,7 +44975,7 @@
       <c r="M432" t="s">
         <v>50</v>
       </c>
-      <c r="O432" s="6">
+      <c r="O432" s="5">
         <f>IF(P432&lt;&gt;"", VLOOKUP(P432, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45041,7 +45041,7 @@
       <c r="M433" t="s">
         <v>50</v>
       </c>
-      <c r="O433" s="6">
+      <c r="O433" s="5">
         <f>IF(P433&lt;&gt;"", VLOOKUP(P433, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45107,7 +45107,7 @@
       <c r="M434" t="s">
         <v>50</v>
       </c>
-      <c r="O434" s="6">
+      <c r="O434" s="5">
         <f>IF(P434&lt;&gt;"", VLOOKUP(P434, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45176,7 +45176,7 @@
       <c r="N435" t="s">
         <v>28</v>
       </c>
-      <c r="O435" s="6">
+      <c r="O435" s="5">
         <f>IF(P435&lt;&gt;"", VLOOKUP(P435, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -45239,7 +45239,7 @@
       <c r="M436" t="s">
         <v>50</v>
       </c>
-      <c r="O436" s="6">
+      <c r="O436" s="5">
         <f>IF(P436&lt;&gt;"", VLOOKUP(P436, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45308,7 +45308,7 @@
       <c r="N437" t="s">
         <v>28</v>
       </c>
-      <c r="O437" s="6">
+      <c r="O437" s="5">
         <f>IF(P437&lt;&gt;"", VLOOKUP(P437, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -45377,7 +45377,7 @@
       <c r="M438" t="s">
         <v>50</v>
       </c>
-      <c r="O438" s="6">
+      <c r="O438" s="5">
         <f>IF(P438&lt;&gt;"", VLOOKUP(P438, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45443,7 +45443,7 @@
       <c r="M439" t="s">
         <v>50</v>
       </c>
-      <c r="O439" s="6">
+      <c r="O439" s="5">
         <f>IF(P439&lt;&gt;"", VLOOKUP(P439, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45503,7 +45503,7 @@
       <c r="M440" t="s">
         <v>50</v>
       </c>
-      <c r="O440" s="6">
+      <c r="O440" s="5">
         <f>IF(P440&lt;&gt;"", VLOOKUP(P440, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45569,7 +45569,7 @@
       <c r="M441" t="s">
         <v>50</v>
       </c>
-      <c r="O441" s="6">
+      <c r="O441" s="5">
         <f>IF(P441&lt;&gt;"", VLOOKUP(P441, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45629,7 +45629,7 @@
       <c r="M442" t="s">
         <v>50</v>
       </c>
-      <c r="O442" s="6">
+      <c r="O442" s="5">
         <f>IF(P442&lt;&gt;"", VLOOKUP(P442, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45689,7 +45689,7 @@
       <c r="M443" t="s">
         <v>50</v>
       </c>
-      <c r="O443" s="6">
+      <c r="O443" s="5">
         <f>IF(P443&lt;&gt;"", VLOOKUP(P443, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45758,7 +45758,7 @@
       <c r="N444" t="s">
         <v>28</v>
       </c>
-      <c r="O444" s="6">
+      <c r="O444" s="5">
         <f>IF(P444&lt;&gt;"", VLOOKUP(P444, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -45827,7 +45827,7 @@
       <c r="M445" t="s">
         <v>50</v>
       </c>
-      <c r="O445" s="6">
+      <c r="O445" s="5">
         <f>IF(P445&lt;&gt;"", VLOOKUP(P445, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45887,7 +45887,7 @@
       <c r="M446" t="s">
         <v>50</v>
       </c>
-      <c r="O446" s="6">
+      <c r="O446" s="5">
         <f>IF(P446&lt;&gt;"", VLOOKUP(P446, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -45956,7 +45956,7 @@
       <c r="N447" t="s">
         <v>28</v>
       </c>
-      <c r="O447" s="6">
+      <c r="O447" s="5">
         <f>IF(P447&lt;&gt;"", VLOOKUP(P447, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -46025,7 +46025,7 @@
       <c r="M448" t="s">
         <v>50</v>
       </c>
-      <c r="O448" s="6">
+      <c r="O448" s="5">
         <f>IF(P448&lt;&gt;"", VLOOKUP(P448, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46091,7 +46091,7 @@
       <c r="M449" t="s">
         <v>50</v>
       </c>
-      <c r="O449" s="6">
+      <c r="O449" s="5">
         <f>IF(P449&lt;&gt;"", VLOOKUP(P449, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46157,7 +46157,7 @@
       <c r="M450" t="s">
         <v>50</v>
       </c>
-      <c r="O450" s="6">
+      <c r="O450" s="5">
         <f>IF(P450&lt;&gt;"", VLOOKUP(P450, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46217,7 +46217,7 @@
       <c r="M451" t="s">
         <v>50</v>
       </c>
-      <c r="O451" s="6">
+      <c r="O451" s="5">
         <f>IF(P451&lt;&gt;"", VLOOKUP(P451, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46283,7 +46283,7 @@
       <c r="M452" t="s">
         <v>50</v>
       </c>
-      <c r="O452" s="6">
+      <c r="O452" s="5">
         <f>IF(P452&lt;&gt;"", VLOOKUP(P452, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46343,7 +46343,7 @@
       <c r="M453" t="s">
         <v>50</v>
       </c>
-      <c r="O453" s="6">
+      <c r="O453" s="5">
         <f>IF(P453&lt;&gt;"", VLOOKUP(P453, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46403,7 +46403,7 @@
       <c r="M454" t="s">
         <v>25</v>
       </c>
-      <c r="O454" s="6">
+      <c r="O454" s="5">
         <f>IF(P454&lt;&gt;"", VLOOKUP(P454, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -46466,7 +46466,7 @@
       <c r="M455" t="s">
         <v>50</v>
       </c>
-      <c r="O455" s="6">
+      <c r="O455" s="5">
         <f>IF(P455&lt;&gt;"", VLOOKUP(P455, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46535,7 +46535,7 @@
       <c r="N456" t="s">
         <v>68</v>
       </c>
-      <c r="O456" s="6">
+      <c r="O456" s="5">
         <f>IF(P456&lt;&gt;"", VLOOKUP(P456, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -46604,7 +46604,7 @@
       <c r="M457" t="s">
         <v>50</v>
       </c>
-      <c r="O457" s="6">
+      <c r="O457" s="5">
         <f>IF(P457&lt;&gt;"", VLOOKUP(P457, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46670,7 +46670,7 @@
       <c r="M458" t="s">
         <v>50</v>
       </c>
-      <c r="O458" s="6">
+      <c r="O458" s="5">
         <f>IF(P458&lt;&gt;"", VLOOKUP(P458, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46736,7 +46736,7 @@
       <c r="M459" t="s">
         <v>50</v>
       </c>
-      <c r="O459" s="6">
+      <c r="O459" s="5">
         <f>IF(P459&lt;&gt;"", VLOOKUP(P459, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46802,7 +46802,7 @@
       <c r="M460" t="s">
         <v>50</v>
       </c>
-      <c r="O460" s="6">
+      <c r="O460" s="5">
         <f>IF(P460&lt;&gt;"", VLOOKUP(P460, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -46862,7 +46862,7 @@
       <c r="M461" t="s">
         <v>25</v>
       </c>
-      <c r="O461" s="6">
+      <c r="O461" s="5">
         <f>IF(P461&lt;&gt;"", VLOOKUP(P461, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -46925,7 +46925,7 @@
       <c r="M462" t="s">
         <v>25</v>
       </c>
-      <c r="O462" s="6">
+      <c r="O462" s="5">
         <f>IF(P462&lt;&gt;"", VLOOKUP(P462, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -46994,7 +46994,7 @@
       <c r="M463" t="s">
         <v>50</v>
       </c>
-      <c r="O463" s="6">
+      <c r="O463" s="5">
         <f>IF(P463&lt;&gt;"", VLOOKUP(P463, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47054,7 +47054,7 @@
       <c r="M464" t="s">
         <v>50</v>
       </c>
-      <c r="O464" s="6">
+      <c r="O464" s="5">
         <f>IF(P464&lt;&gt;"", VLOOKUP(P464, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47123,7 +47123,7 @@
       <c r="N465" t="s">
         <v>28</v>
       </c>
-      <c r="O465" s="6">
+      <c r="O465" s="5">
         <f>IF(P465&lt;&gt;"", VLOOKUP(P465, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>4</v>
       </c>
@@ -47192,7 +47192,7 @@
       <c r="M466" t="s">
         <v>50</v>
       </c>
-      <c r="O466" s="6">
+      <c r="O466" s="5">
         <f>IF(P466&lt;&gt;"", VLOOKUP(P466, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47261,7 +47261,7 @@
       <c r="N467" t="s">
         <v>28</v>
       </c>
-      <c r="O467" s="6">
+      <c r="O467" s="5">
         <f>IF(P467&lt;&gt;"", VLOOKUP(P467, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -47324,7 +47324,7 @@
       <c r="M468" t="s">
         <v>50</v>
       </c>
-      <c r="O468" s="6">
+      <c r="O468" s="5">
         <f>IF(P468&lt;&gt;"", VLOOKUP(P468, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47384,7 +47384,7 @@
       <c r="M469" t="s">
         <v>50</v>
       </c>
-      <c r="O469" s="6">
+      <c r="O469" s="5">
         <f>IF(P469&lt;&gt;"", VLOOKUP(P469, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47444,7 +47444,7 @@
       <c r="M470" t="s">
         <v>50</v>
       </c>
-      <c r="O470" s="6">
+      <c r="O470" s="5">
         <f>IF(P470&lt;&gt;"", VLOOKUP(P470, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47504,7 +47504,7 @@
       <c r="M471" t="s">
         <v>50</v>
       </c>
-      <c r="O471" s="6">
+      <c r="O471" s="5">
         <f>IF(P471&lt;&gt;"", VLOOKUP(P471, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47564,7 +47564,7 @@
       <c r="M472" t="s">
         <v>25</v>
       </c>
-      <c r="O472" s="6">
+      <c r="O472" s="5">
         <f>IF(P472&lt;&gt;"", VLOOKUP(P472, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -47627,7 +47627,7 @@
       <c r="M473" t="s">
         <v>50</v>
       </c>
-      <c r="O473" s="6">
+      <c r="O473" s="5">
         <f>IF(P473&lt;&gt;"", VLOOKUP(P473, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47693,7 +47693,7 @@
       <c r="M474" t="s">
         <v>50</v>
       </c>
-      <c r="O474" s="6">
+      <c r="O474" s="5">
         <f>IF(P474&lt;&gt;"", VLOOKUP(P474, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47759,7 +47759,7 @@
       <c r="M475" t="s">
         <v>50</v>
       </c>
-      <c r="O475" s="6">
+      <c r="O475" s="5">
         <f>IF(P475&lt;&gt;"", VLOOKUP(P475, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -47828,7 +47828,7 @@
       <c r="N476" t="s">
         <v>28</v>
       </c>
-      <c r="O476" s="6">
+      <c r="O476" s="5">
         <f>IF(P476&lt;&gt;"", VLOOKUP(P476, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>3</v>
       </c>
@@ -47900,7 +47900,7 @@
       <c r="N477" t="s">
         <v>68</v>
       </c>
-      <c r="O477" s="6">
+      <c r="O477" s="5">
         <f>IF(P477&lt;&gt;"", VLOOKUP(P477, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -47969,7 +47969,7 @@
       <c r="M478" t="s">
         <v>50</v>
       </c>
-      <c r="O478" s="6">
+      <c r="O478" s="5">
         <f>IF(P478&lt;&gt;"", VLOOKUP(P478, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -48032,7 +48032,7 @@
       <c r="M479" t="s">
         <v>25</v>
       </c>
-      <c r="O479" s="6">
+      <c r="O479" s="5">
         <f>IF(P479&lt;&gt;"", VLOOKUP(P479, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -48104,7 +48104,7 @@
       <c r="N480" t="s">
         <v>28</v>
       </c>
-      <c r="O480" s="6">
+      <c r="O480" s="5">
         <f>IF(P480&lt;&gt;"", VLOOKUP(P480, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -48176,7 +48176,7 @@
       <c r="N481" t="s">
         <v>28</v>
       </c>
-      <c r="O481" s="6">
+      <c r="O481" s="5">
         <f>IF(P481&lt;&gt;"", VLOOKUP(P481, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -48248,7 +48248,7 @@
       <c r="N482" t="s">
         <v>68</v>
       </c>
-      <c r="O482" s="6">
+      <c r="O482" s="5">
         <f>IF(P482&lt;&gt;"", VLOOKUP(P482, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -48320,7 +48320,7 @@
       <c r="N483" t="s">
         <v>28</v>
       </c>
-      <c r="O483" s="6">
+      <c r="O483" s="5">
         <f>IF(P483&lt;&gt;"", VLOOKUP(P483, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -48389,7 +48389,7 @@
       <c r="M484" t="s">
         <v>50</v>
       </c>
-      <c r="O484" s="6">
+      <c r="O484" s="5">
         <f>IF(P484&lt;&gt;"", VLOOKUP(P484, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -48458,7 +48458,7 @@
       <c r="N485" t="s">
         <v>68</v>
       </c>
-      <c r="O485" s="6">
+      <c r="O485" s="5">
         <f>IF(P485&lt;&gt;"", VLOOKUP(P485, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -48530,7 +48530,7 @@
       <c r="N486" t="s">
         <v>28</v>
       </c>
-      <c r="O486" s="6">
+      <c r="O486" s="5">
         <f>IF(P486&lt;&gt;"", VLOOKUP(P486, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -48602,7 +48602,7 @@
       <c r="N487" t="s">
         <v>28</v>
       </c>
-      <c r="O487" s="6">
+      <c r="O487" s="5">
         <f>IF(P487&lt;&gt;"", VLOOKUP(P487, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -48665,7 +48665,7 @@
       <c r="M488" t="s">
         <v>25</v>
       </c>
-      <c r="O488" s="6">
+      <c r="O488" s="5">
         <f>IF(P488&lt;&gt;"", VLOOKUP(P488, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -48737,7 +48737,7 @@
       <c r="N489" t="s">
         <v>28</v>
       </c>
-      <c r="O489" s="6">
+      <c r="O489" s="5">
         <f>IF(P489&lt;&gt;"", VLOOKUP(P489, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -48806,7 +48806,7 @@
       <c r="M490" t="s">
         <v>50</v>
       </c>
-      <c r="O490" s="6">
+      <c r="O490" s="5">
         <f>IF(P490&lt;&gt;"", VLOOKUP(P490, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -48872,7 +48872,7 @@
       <c r="M491" t="s">
         <v>50</v>
       </c>
-      <c r="O491" s="6">
+      <c r="O491" s="5">
         <f>IF(P491&lt;&gt;"", VLOOKUP(P491, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -48932,7 +48932,7 @@
       <c r="M492" t="s">
         <v>50</v>
       </c>
-      <c r="O492" s="6">
+      <c r="O492" s="5">
         <f>IF(P492&lt;&gt;"", VLOOKUP(P492, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49001,7 +49001,7 @@
       <c r="N493" t="s">
         <v>28</v>
       </c>
-      <c r="O493" s="6">
+      <c r="O493" s="5">
         <f>IF(P493&lt;&gt;"", VLOOKUP(P493, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -49070,7 +49070,7 @@
       <c r="M494" t="s">
         <v>50</v>
       </c>
-      <c r="O494" s="6">
+      <c r="O494" s="5">
         <f>IF(P494&lt;&gt;"", VLOOKUP(P494, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49136,7 +49136,7 @@
       <c r="M495" t="s">
         <v>50</v>
       </c>
-      <c r="O495" s="6">
+      <c r="O495" s="5">
         <f>IF(P495&lt;&gt;"", VLOOKUP(P495, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49205,7 +49205,7 @@
       <c r="N496" t="s">
         <v>28</v>
       </c>
-      <c r="O496" s="6">
+      <c r="O496" s="5">
         <f>IF(P496&lt;&gt;"", VLOOKUP(P496, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>1</v>
       </c>
@@ -49277,7 +49277,7 @@
       <c r="N497" t="s">
         <v>28</v>
       </c>
-      <c r="O497" s="6">
+      <c r="O497" s="5">
         <f>IF(P497&lt;&gt;"", VLOOKUP(P497, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -49346,7 +49346,7 @@
       <c r="M498" t="s">
         <v>50</v>
       </c>
-      <c r="O498" s="6">
+      <c r="O498" s="5">
         <f>IF(P498&lt;&gt;"", VLOOKUP(P498, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49406,7 +49406,7 @@
       <c r="M499" t="s">
         <v>50</v>
       </c>
-      <c r="O499" s="6">
+      <c r="O499" s="5">
         <f>IF(P499&lt;&gt;"", VLOOKUP(P499, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49475,7 +49475,7 @@
       <c r="N500" t="s">
         <v>119</v>
       </c>
-      <c r="O500" s="6">
+      <c r="O500" s="5">
         <f>IF(P500&lt;&gt;"", VLOOKUP(P500, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>2</v>
       </c>
@@ -49538,7 +49538,7 @@
       <c r="M501" t="s">
         <v>50</v>
       </c>
-      <c r="O501" s="6">
+      <c r="O501" s="5">
         <f>IF(P501&lt;&gt;"", VLOOKUP(P501, lookup!$A:$B, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
@@ -49642,7 +49642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C99BD53-8C9E-43E0-BB52-ACC46E848327}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>